<commit_message>
Networking added to docs
</commit_message>
<xml_diff>
--- a/ReleaseTimelines.xlsx
+++ b/ReleaseTimelines.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="88">
   <si>
     <t>Dev</t>
   </si>
@@ -41,24 +41,12 @@
     <t>Business</t>
   </si>
   <si>
-    <t>Hosting</t>
-  </si>
-  <si>
     <t>End User</t>
   </si>
   <si>
     <t>Mainframe Software</t>
   </si>
   <si>
-    <t>Basic</t>
-  </si>
-  <si>
-    <t>Game</t>
-  </si>
-  <si>
-    <t>Adventure</t>
-  </si>
-  <si>
     <t>Branch</t>
   </si>
   <si>
@@ -101,24 +89,9 @@
     <t>QA</t>
   </si>
   <si>
-    <t>Text Based</t>
-  </si>
-  <si>
-    <t>Platformer</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
     <t>Office</t>
   </si>
   <si>
-    <t>Text Editor</t>
-  </si>
-  <si>
-    <t>Mainframe</t>
-  </si>
-  <si>
     <t>Dev Tooling</t>
   </si>
   <si>
@@ -203,12 +176,6 @@
     <t>Transactions</t>
   </si>
   <si>
-    <t>Business Hosting</t>
-  </si>
-  <si>
-    <t>Multi-tenancy</t>
-  </si>
-  <si>
     <t>Compiler</t>
   </si>
   <si>
@@ -282,6 +249,45 @@
   </si>
   <si>
     <t>Remote Support</t>
+  </si>
+  <si>
+    <t>ARPANET 50 Kbps</t>
+  </si>
+  <si>
+    <t>NSFNET 56 Kbps</t>
+  </si>
+  <si>
+    <t>NSFNET 45 Mbps</t>
+  </si>
+  <si>
+    <t>NSFNET 145 Mbps</t>
+  </si>
+  <si>
+    <t>Specialist</t>
+  </si>
+  <si>
+    <t>Dial-up 56 Kbps</t>
+  </si>
+  <si>
+    <t>Consumer</t>
+  </si>
+  <si>
+    <t>Cable 1 Mbps</t>
+  </si>
+  <si>
+    <t>DSL 100 Kps</t>
+  </si>
+  <si>
+    <t>Fibre 25 Mbps</t>
+  </si>
+  <si>
+    <t>Cable 10 Mbps</t>
+  </si>
+  <si>
+    <t>Fibre 100 Mbps</t>
+  </si>
+  <si>
+    <t>Fibre 1 Gbps</t>
   </si>
 </sst>
 </file>
@@ -297,7 +303,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,7 +348,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -359,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -373,9 +397,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,13 +685,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE75"/>
+  <dimension ref="A1:BE84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="AD24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E49" sqref="E49"/>
+      <selection pane="bottomRight" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,22 +704,22 @@
   <sheetData>
     <row r="1" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -914,10 +943,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -970,7 +999,7 @@
       <c r="BC3" s="2"/>
       <c r="BD3" s="2"/>
       <c r="BE3" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:57" x14ac:dyDescent="0.25">
@@ -979,10 +1008,10 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -1030,7 +1059,7 @@
       <c r="BC4" s="2"/>
       <c r="BD4" s="2"/>
       <c r="BE4" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:57" x14ac:dyDescent="0.25">
@@ -1039,10 +1068,10 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
@@ -1085,7 +1114,7 @@
       <c r="BC5" s="2"/>
       <c r="BD5" s="2"/>
       <c r="BE5" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:57" x14ac:dyDescent="0.25">
@@ -1094,10 +1123,10 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
@@ -1135,7 +1164,7 @@
       <c r="BC6" s="2"/>
       <c r="BD6" s="2"/>
       <c r="BE6" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:57" x14ac:dyDescent="0.25">
@@ -1144,10 +1173,10 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
@@ -1185,7 +1214,7 @@
       <c r="BC7" s="2"/>
       <c r="BD7" s="2"/>
       <c r="BE7" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:57" x14ac:dyDescent="0.25">
@@ -1194,10 +1223,10 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
@@ -1230,7 +1259,7 @@
       <c r="BC8" s="2"/>
       <c r="BD8" s="2"/>
       <c r="BE8" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:57" x14ac:dyDescent="0.25">
@@ -1239,10 +1268,10 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
@@ -1275,7 +1304,7 @@
       <c r="BC9" s="2"/>
       <c r="BD9" s="2"/>
       <c r="BE9" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:57" x14ac:dyDescent="0.25">
@@ -1284,10 +1313,10 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="AE10" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
@@ -1315,7 +1344,7 @@
       <c r="BC10" s="2"/>
       <c r="BD10" s="2"/>
       <c r="BE10" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:57" x14ac:dyDescent="0.25">
@@ -1324,10 +1353,10 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="AJ11" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AK11" s="2"/>
       <c r="AL11" s="2"/>
@@ -1350,7 +1379,7 @@
       <c r="BC11" s="2"/>
       <c r="BD11" s="2"/>
       <c r="BE11" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:57" x14ac:dyDescent="0.25">
@@ -1359,10 +1388,10 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="AJ12" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AK12" s="2"/>
       <c r="AL12" s="2"/>
@@ -1385,7 +1414,7 @@
       <c r="BC12" s="2"/>
       <c r="BD12" s="2"/>
       <c r="BE12" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:57" x14ac:dyDescent="0.25">
@@ -1394,10 +1423,10 @@
         <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="AO13" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AP13" s="2"/>
       <c r="AQ13" s="2"/>
@@ -1415,7 +1444,7 @@
       <c r="BC13" s="2"/>
       <c r="BD13" s="2"/>
       <c r="BE13" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:57" x14ac:dyDescent="0.25">
@@ -1424,10 +1453,10 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="AO14" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AP14" s="2"/>
       <c r="AQ14" s="2"/>
@@ -1445,7 +1474,7 @@
       <c r="BC14" s="2"/>
       <c r="BD14" s="2"/>
       <c r="BE14" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:57" x14ac:dyDescent="0.25">
@@ -1454,10 +1483,10 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AT15" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AU15" s="2"/>
       <c r="AV15" s="2"/>
@@ -1470,7 +1499,7 @@
       <c r="BC15" s="2"/>
       <c r="BD15" s="2"/>
       <c r="BE15" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:57" x14ac:dyDescent="0.25">
@@ -1479,7 +1508,7 @@
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="AT16" s="5"/>
       <c r="AU16" s="5"/>
@@ -1487,7 +1516,7 @@
       <c r="AW16" s="5"/>
       <c r="AX16" s="5"/>
       <c r="AY16" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AZ16" s="2"/>
       <c r="BA16" s="2"/>
@@ -1495,7 +1524,7 @@
       <c r="BC16" s="2"/>
       <c r="BD16" s="2"/>
       <c r="BE16" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:57" x14ac:dyDescent="0.25">
@@ -1504,28 +1533,28 @@
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="BD17" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="BE17" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
@@ -1568,7 +1597,7 @@
       <c r="BC18" s="3"/>
       <c r="BD18" s="3"/>
       <c r="BE18" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:57" x14ac:dyDescent="0.25">
@@ -1577,10 +1606,10 @@
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="U19" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
@@ -1618,7 +1647,7 @@
       <c r="BC19" s="3"/>
       <c r="BD19" s="3"/>
       <c r="BE19" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:57" x14ac:dyDescent="0.25">
@@ -1627,10 +1656,10 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="Z20" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AA20" s="3"/>
       <c r="AB20" s="3"/>
@@ -1663,7 +1692,7 @@
       <c r="BC20" s="3"/>
       <c r="BD20" s="3"/>
       <c r="BE20" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:57" x14ac:dyDescent="0.25">
@@ -1672,10 +1701,10 @@
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="AE21" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AF21" s="3"/>
       <c r="AG21" s="3"/>
@@ -1703,7 +1732,7 @@
       <c r="BC21" s="3"/>
       <c r="BD21" s="3"/>
       <c r="BE21" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:57" x14ac:dyDescent="0.25">
@@ -1712,10 +1741,10 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="AJ22" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AK22" s="3"/>
       <c r="AL22" s="3"/>
@@ -1738,7 +1767,7 @@
       <c r="BC22" s="3"/>
       <c r="BD22" s="3"/>
       <c r="BE22" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:57" x14ac:dyDescent="0.25">
@@ -1747,10 +1776,10 @@
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="AO23" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AP23" s="3"/>
       <c r="AQ23" s="3"/>
@@ -1768,7 +1797,7 @@
       <c r="BC23" s="3"/>
       <c r="BD23" s="3"/>
       <c r="BE23" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:57" x14ac:dyDescent="0.25">
@@ -1777,10 +1806,10 @@
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="AT24" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AU24" s="3"/>
       <c r="AV24" s="3"/>
@@ -1793,7 +1822,7 @@
       <c r="BC24" s="3"/>
       <c r="BD24" s="3"/>
       <c r="BE24" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:57" x14ac:dyDescent="0.25">
@@ -1802,10 +1831,10 @@
         <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="AY25" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AZ25" s="3"/>
       <c r="BA25" s="3"/>
@@ -1813,7 +1842,7 @@
       <c r="BC25" s="3"/>
       <c r="BD25" s="3"/>
       <c r="BE25" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:57" x14ac:dyDescent="0.25">
@@ -1822,7 +1851,7 @@
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="AY26" s="5"/>
       <c r="AZ26" s="5"/>
@@ -1830,10 +1859,10 @@
       <c r="BB26" s="5"/>
       <c r="BC26" s="5"/>
       <c r="BD26" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="BE26" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:57" x14ac:dyDescent="0.25">
@@ -1845,10 +1874,10 @@
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
@@ -1891,7 +1920,7 @@
       <c r="BC27" s="4"/>
       <c r="BD27" s="4"/>
       <c r="BE27" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:57" x14ac:dyDescent="0.25">
@@ -1900,10 +1929,10 @@
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="U28" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="V28" s="4"/>
       <c r="W28" s="4"/>
@@ -1941,7 +1970,7 @@
       <c r="BC28" s="4"/>
       <c r="BD28" s="4"/>
       <c r="BE28" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:57" x14ac:dyDescent="0.25">
@@ -1950,10 +1979,10 @@
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="Z29" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AA29" s="4"/>
       <c r="AB29" s="4"/>
@@ -1986,7 +2015,7 @@
       <c r="BC29" s="4"/>
       <c r="BD29" s="4"/>
       <c r="BE29" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:57" x14ac:dyDescent="0.25">
@@ -1995,10 +2024,10 @@
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="AE30" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AF30" s="4"/>
       <c r="AG30" s="4"/>
@@ -2026,7 +2055,7 @@
       <c r="BC30" s="4"/>
       <c r="BD30" s="4"/>
       <c r="BE30" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:57" x14ac:dyDescent="0.25">
@@ -2035,10 +2064,10 @@
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="AJ31" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AK31" s="4"/>
       <c r="AL31" s="4"/>
@@ -2061,7 +2090,7 @@
       <c r="BC31" s="4"/>
       <c r="BD31" s="4"/>
       <c r="BE31" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:57" x14ac:dyDescent="0.25">
@@ -2070,10 +2099,10 @@
         <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="AO32" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AP32" s="4"/>
       <c r="AQ32" s="4"/>
@@ -2091,7 +2120,7 @@
       <c r="BC32" s="4"/>
       <c r="BD32" s="4"/>
       <c r="BE32" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:57" x14ac:dyDescent="0.25">
@@ -2100,10 +2129,10 @@
         <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="AT33" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AU33" s="4"/>
       <c r="AV33" s="4"/>
@@ -2116,24 +2145,24 @@
       <c r="BC33" s="4"/>
       <c r="BD33" s="4"/>
       <c r="BE33" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D34">
         <v>2</v>
       </c>
       <c r="E34" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
@@ -2186,19 +2215,19 @@
       <c r="BC34" s="6"/>
       <c r="BD34" s="6"/>
       <c r="BE34" s="6" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
+      <c r="A35" s="10"/>
       <c r="D35">
         <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
@@ -2246,19 +2275,19 @@
       <c r="BC35" s="6"/>
       <c r="BD35" s="6"/>
       <c r="BE35" s="6" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
+      <c r="A36" s="10"/>
       <c r="D36">
         <v>3</v>
       </c>
       <c r="E36" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="P36" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="Q36" s="6"/>
       <c r="R36" s="6"/>
@@ -2301,19 +2330,19 @@
       <c r="BC36" s="6"/>
       <c r="BD36" s="6"/>
       <c r="BE36" s="6" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
+      <c r="A37" s="10"/>
       <c r="D37">
         <v>3</v>
       </c>
       <c r="E37" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="U37" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="V37" s="6"/>
       <c r="W37" s="6"/>
@@ -2351,19 +2380,19 @@
       <c r="BC37" s="6"/>
       <c r="BD37" s="6"/>
       <c r="BE37" s="6" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
+      <c r="A38" s="10"/>
       <c r="D38">
         <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="Z38" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AA38" s="6"/>
       <c r="AB38" s="6"/>
@@ -2396,19 +2425,19 @@
       <c r="BC38" s="6"/>
       <c r="BD38" s="6"/>
       <c r="BE38" s="6" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
+      <c r="A39" s="10"/>
       <c r="D39">
         <v>3</v>
       </c>
       <c r="E39" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="AE39" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AF39" s="6"/>
       <c r="AG39" s="6"/>
@@ -2436,19 +2465,19 @@
       <c r="BC39" s="6"/>
       <c r="BD39" s="6"/>
       <c r="BE39" s="6" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
+      <c r="A40" s="10"/>
       <c r="D40">
         <v>3</v>
       </c>
       <c r="E40" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="AJ40" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AK40" s="6"/>
       <c r="AL40" s="6"/>
@@ -2471,19 +2500,19 @@
       <c r="BC40" s="6"/>
       <c r="BD40" s="6"/>
       <c r="BE40" s="6" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
+      <c r="A41" s="10"/>
       <c r="D41">
         <v>3</v>
       </c>
       <c r="E41" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="AO41" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AP41" s="6"/>
       <c r="AQ41" s="6"/>
@@ -2501,19 +2530,19 @@
       <c r="BC41" s="6"/>
       <c r="BD41" s="6"/>
       <c r="BE41" s="6" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
+      <c r="A42" s="10"/>
       <c r="D42">
         <v>4</v>
       </c>
       <c r="E42" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="AT42" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AU42" s="6"/>
       <c r="AV42" s="6"/>
@@ -2526,23 +2555,23 @@
       <c r="BC42" s="6"/>
       <c r="BD42" s="6"/>
       <c r="BE42" s="6" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
+      <c r="A43" s="10"/>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D43">
         <f>D34+1</f>
         <v>3</v>
       </c>
       <c r="E43" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="P43" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="Q43" s="7"/>
       <c r="R43" s="7"/>
@@ -2585,20 +2614,20 @@
       <c r="BC43" s="7"/>
       <c r="BD43" s="7"/>
       <c r="BE43" s="7" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
+      <c r="A44" s="10"/>
       <c r="D44">
-        <f t="shared" ref="D44:D49" si="0">D35+1</f>
+        <f t="shared" ref="D44:D48" si="0">D35+1</f>
         <v>3</v>
       </c>
       <c r="E44" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="U44" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="V44" s="7"/>
       <c r="W44" s="7"/>
@@ -2636,20 +2665,20 @@
       <c r="BC44" s="7"/>
       <c r="BD44" s="7"/>
       <c r="BE44" s="7" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A45" s="9"/>
+      <c r="A45" s="10"/>
       <c r="D45">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E45" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="Z45" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AA45" s="7"/>
       <c r="AB45" s="7"/>
@@ -2682,20 +2711,20 @@
       <c r="BC45" s="7"/>
       <c r="BD45" s="7"/>
       <c r="BE45" s="7" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
+      <c r="A46" s="10"/>
       <c r="D46">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E46" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="AE46" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AF46" s="7"/>
       <c r="AG46" s="7"/>
@@ -2723,20 +2752,20 @@
       <c r="BC46" s="7"/>
       <c r="BD46" s="7"/>
       <c r="BE46" s="7" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A47" s="9"/>
+      <c r="A47" s="10"/>
       <c r="D47">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E47" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="AJ47" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AK47" s="7"/>
       <c r="AL47" s="7"/>
@@ -2759,20 +2788,20 @@
       <c r="BC47" s="7"/>
       <c r="BD47" s="7"/>
       <c r="BE47" s="7" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
+      <c r="A48" s="10"/>
       <c r="D48">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E48" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="AO48" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AP48" s="7"/>
       <c r="AQ48" s="7"/>
@@ -2790,20 +2819,19 @@
       <c r="BC48" s="7"/>
       <c r="BD48" s="7"/>
       <c r="BE48" s="7" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A49" s="9"/>
+      <c r="A49" s="10"/>
       <c r="D49">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E49">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="E49" t="s">
+        <v>70</v>
       </c>
       <c r="AT49" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AU49" s="7"/>
       <c r="AV49" s="7"/>
@@ -2816,332 +2844,959 @@
       <c r="BC49" s="7"/>
       <c r="BD49" s="7"/>
       <c r="BE49" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A50" s="11"/>
+      <c r="B50" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" t="s">
+        <v>79</v>
+      </c>
+      <c r="E50" t="s">
+        <v>75</v>
+      </c>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="5"/>
+      <c r="P50" s="5"/>
+      <c r="Q50" s="5"/>
+      <c r="R50" s="5"/>
+      <c r="S50" s="5"/>
+      <c r="T50" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="U50" s="12"/>
+      <c r="V50" s="12"/>
+      <c r="W50" s="12"/>
+      <c r="X50" s="12"/>
+      <c r="Y50" s="12"/>
+      <c r="Z50" s="12"/>
+      <c r="AA50" s="12"/>
+      <c r="AB50" s="12"/>
+      <c r="AC50" s="12"/>
+      <c r="AD50" s="12"/>
+      <c r="AE50" s="12"/>
+      <c r="AF50" s="12"/>
+      <c r="AG50" s="12"/>
+      <c r="AH50" s="12"/>
+      <c r="AI50" s="12"/>
+      <c r="AJ50" s="12"/>
+      <c r="AK50" s="12"/>
+      <c r="AL50" s="12"/>
+      <c r="AM50" s="12"/>
+      <c r="AN50" s="12"/>
+      <c r="AO50" s="12"/>
+      <c r="AP50" s="12"/>
+      <c r="AQ50" s="12"/>
+      <c r="AR50" s="12"/>
+      <c r="AS50" s="12"/>
+      <c r="AT50" s="12"/>
+      <c r="AU50" s="12"/>
+      <c r="AV50" s="12"/>
+      <c r="AW50" s="12"/>
+      <c r="AX50" s="12"/>
+      <c r="AY50" s="12"/>
+      <c r="AZ50" s="12"/>
+      <c r="BA50" s="12"/>
+      <c r="BB50" s="12"/>
+      <c r="BC50" s="12"/>
+      <c r="BD50" s="12"/>
+      <c r="BE50" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A51" s="11"/>
+      <c r="E51" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="50" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="5"/>
+      <c r="P51" s="5"/>
+      <c r="Q51" s="5"/>
+      <c r="R51" s="5"/>
+      <c r="S51" s="5"/>
+      <c r="T51" s="5"/>
+      <c r="U51" s="5"/>
+      <c r="V51" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="W51" s="12"/>
+      <c r="X51" s="12"/>
+      <c r="Y51" s="12"/>
+      <c r="Z51" s="12"/>
+      <c r="AA51" s="12"/>
+      <c r="AB51" s="12"/>
+      <c r="AC51" s="12"/>
+      <c r="AD51" s="12"/>
+      <c r="AE51" s="12"/>
+      <c r="AF51" s="12"/>
+      <c r="AG51" s="12"/>
+      <c r="AH51" s="12"/>
+      <c r="AI51" s="12"/>
+      <c r="AJ51" s="12"/>
+      <c r="AK51" s="12"/>
+      <c r="AL51" s="12"/>
+      <c r="AM51" s="12"/>
+      <c r="AN51" s="12"/>
+      <c r="AO51" s="12"/>
+      <c r="AP51" s="12"/>
+      <c r="AQ51" s="12"/>
+      <c r="AR51" s="12"/>
+      <c r="AS51" s="12"/>
+      <c r="AT51" s="12"/>
+      <c r="AU51" s="12"/>
+      <c r="AV51" s="12"/>
+      <c r="AW51" s="12"/>
+      <c r="AX51" s="12"/>
+      <c r="AY51" s="12"/>
+      <c r="AZ51" s="12"/>
+      <c r="BA51" s="12"/>
+      <c r="BB51" s="12"/>
+      <c r="BC51" s="12"/>
+      <c r="BD51" s="12"/>
+      <c r="BE51" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A52" s="11"/>
+      <c r="E52" t="s">
+        <v>77</v>
+      </c>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5"/>
+      <c r="N52" s="5"/>
+      <c r="O52" s="5"/>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
+      <c r="R52" s="5"/>
+      <c r="S52" s="5"/>
+      <c r="T52" s="5"/>
+      <c r="U52" s="5"/>
+      <c r="V52" s="5"/>
+      <c r="W52" s="5"/>
+      <c r="X52" s="5"/>
+      <c r="Y52" s="5"/>
+      <c r="Z52" s="5"/>
+      <c r="AA52" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB52" s="12"/>
+      <c r="AC52" s="12"/>
+      <c r="AD52" s="12"/>
+      <c r="AE52" s="12"/>
+      <c r="AF52" s="12"/>
+      <c r="AG52" s="12"/>
+      <c r="AH52" s="12"/>
+      <c r="AI52" s="12"/>
+      <c r="AJ52" s="12"/>
+      <c r="AK52" s="12"/>
+      <c r="AL52" s="12"/>
+      <c r="AM52" s="12"/>
+      <c r="AN52" s="12"/>
+      <c r="AO52" s="12"/>
+      <c r="AP52" s="12"/>
+      <c r="AQ52" s="12"/>
+      <c r="AR52" s="12"/>
+      <c r="AS52" s="12"/>
+      <c r="AT52" s="12"/>
+      <c r="AU52" s="12"/>
+      <c r="AV52" s="12"/>
+      <c r="AW52" s="12"/>
+      <c r="AX52" s="12"/>
+      <c r="AY52" s="12"/>
+      <c r="AZ52" s="12"/>
+      <c r="BA52" s="12"/>
+      <c r="BB52" s="12"/>
+      <c r="BC52" s="12"/>
+      <c r="BD52" s="12"/>
+      <c r="BE52" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A53" s="11"/>
+      <c r="E53" t="s">
+        <v>78</v>
+      </c>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5"/>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+      <c r="R53" s="5"/>
+      <c r="S53" s="5"/>
+      <c r="T53" s="5"/>
+      <c r="U53" s="5"/>
+      <c r="V53" s="5"/>
+      <c r="W53" s="5"/>
+      <c r="X53" s="5"/>
+      <c r="Y53" s="5"/>
+      <c r="Z53" s="5"/>
+      <c r="AA53" s="5"/>
+      <c r="AB53" s="5"/>
+      <c r="AC53" s="5"/>
+      <c r="AD53" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE53" s="12"/>
+      <c r="AF53" s="12"/>
+      <c r="AG53" s="12"/>
+      <c r="AH53" s="12"/>
+      <c r="AI53" s="12"/>
+      <c r="AJ53" s="12"/>
+      <c r="AK53" s="12"/>
+      <c r="AL53" s="12"/>
+      <c r="AM53" s="12"/>
+      <c r="AN53" s="12"/>
+      <c r="AO53" s="12"/>
+      <c r="AP53" s="12"/>
+      <c r="AQ53" s="12"/>
+      <c r="AR53" s="12"/>
+      <c r="AS53" s="12"/>
+      <c r="AT53" s="12"/>
+      <c r="AU53" s="12"/>
+      <c r="AV53" s="12"/>
+      <c r="AW53" s="12"/>
+      <c r="AX53" s="12"/>
+      <c r="AY53" s="12"/>
+      <c r="AZ53" s="12"/>
+      <c r="BA53" s="12"/>
+      <c r="BB53" s="12"/>
+      <c r="BC53" s="12"/>
+      <c r="BD53" s="12"/>
+      <c r="BE53" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A54" s="11"/>
+      <c r="C54" t="s">
+        <v>81</v>
+      </c>
+      <c r="E54" t="s">
+        <v>80</v>
+      </c>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="5"/>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="5"/>
+      <c r="S54" s="5"/>
+      <c r="T54" s="5"/>
+      <c r="U54" s="5"/>
+      <c r="V54" s="5"/>
+      <c r="W54" s="5"/>
+      <c r="X54" s="5"/>
+      <c r="Y54" s="5"/>
+      <c r="Z54" s="5"/>
+      <c r="AA54" s="5"/>
+      <c r="AB54" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC54" s="9"/>
+      <c r="AD54" s="9"/>
+      <c r="AE54" s="9"/>
+      <c r="AF54" s="9"/>
+      <c r="AG54" s="9"/>
+      <c r="AH54" s="9"/>
+      <c r="AI54" s="9"/>
+      <c r="AJ54" s="9"/>
+      <c r="AK54" s="9"/>
+      <c r="AL54" s="9"/>
+      <c r="AM54" s="9"/>
+      <c r="AN54" s="9"/>
+      <c r="AO54" s="9"/>
+      <c r="AP54" s="9"/>
+      <c r="AQ54" s="9"/>
+      <c r="AR54" s="9"/>
+      <c r="AS54" s="9"/>
+      <c r="AT54" s="9"/>
+      <c r="AU54" s="9"/>
+      <c r="AV54" s="9"/>
+      <c r="AW54" s="9"/>
+      <c r="AX54" s="9"/>
+      <c r="AY54" s="9"/>
+      <c r="AZ54" s="9"/>
+      <c r="BA54" s="9"/>
+      <c r="BB54" s="9"/>
+      <c r="BC54" s="9"/>
+      <c r="BD54" s="9"/>
+      <c r="BE54" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A55" s="11"/>
+      <c r="E55" t="s">
+        <v>83</v>
+      </c>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="5"/>
+      <c r="P55" s="5"/>
+      <c r="Q55" s="5"/>
+      <c r="R55" s="5"/>
+      <c r="S55" s="5"/>
+      <c r="T55" s="5"/>
+      <c r="U55" s="5"/>
+      <c r="V55" s="5"/>
+      <c r="W55" s="5"/>
+      <c r="X55" s="5"/>
+      <c r="Y55" s="5"/>
+      <c r="Z55" s="5"/>
+      <c r="AA55" s="5"/>
+      <c r="AB55" s="5"/>
+      <c r="AC55" s="5"/>
+      <c r="AD55" s="5"/>
+      <c r="AE55" s="5"/>
+      <c r="AF55" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG55" s="9"/>
+      <c r="AH55" s="9"/>
+      <c r="AI55" s="9"/>
+      <c r="AJ55" s="9"/>
+      <c r="AK55" s="9"/>
+      <c r="AL55" s="9"/>
+      <c r="AM55" s="9"/>
+      <c r="AN55" s="9"/>
+      <c r="AO55" s="9"/>
+      <c r="AP55" s="9"/>
+      <c r="AQ55" s="9"/>
+      <c r="AR55" s="9"/>
+      <c r="AS55" s="9"/>
+      <c r="AT55" s="9"/>
+      <c r="AU55" s="9"/>
+      <c r="AV55" s="9"/>
+      <c r="AW55" s="9"/>
+      <c r="AX55" s="9"/>
+      <c r="AY55" s="9"/>
+      <c r="AZ55" s="9"/>
+      <c r="BA55" s="9"/>
+      <c r="BB55" s="9"/>
+      <c r="BC55" s="9"/>
+      <c r="BD55" s="9"/>
+      <c r="BE55" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A56" s="11"/>
+      <c r="E56" t="s">
+        <v>82</v>
+      </c>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="5"/>
+      <c r="O56" s="5"/>
+      <c r="P56" s="5"/>
+      <c r="Q56" s="5"/>
+      <c r="R56" s="5"/>
+      <c r="S56" s="5"/>
+      <c r="T56" s="5"/>
+      <c r="U56" s="5"/>
+      <c r="V56" s="5"/>
+      <c r="W56" s="5"/>
+      <c r="X56" s="5"/>
+      <c r="Y56" s="5"/>
+      <c r="Z56" s="5"/>
+      <c r="AA56" s="5"/>
+      <c r="AB56" s="5"/>
+      <c r="AC56" s="5"/>
+      <c r="AD56" s="5"/>
+      <c r="AE56" s="5"/>
+      <c r="AF56" s="5"/>
+      <c r="AG56" s="5"/>
+      <c r="AH56" s="5"/>
+      <c r="AI56" s="5"/>
+      <c r="AJ56" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK56" s="9"/>
+      <c r="AL56" s="9"/>
+      <c r="AM56" s="9"/>
+      <c r="AN56" s="9"/>
+      <c r="AO56" s="9"/>
+      <c r="AP56" s="9"/>
+      <c r="AQ56" s="9"/>
+      <c r="AR56" s="9"/>
+      <c r="AS56" s="9"/>
+      <c r="AT56" s="9"/>
+      <c r="AU56" s="9"/>
+      <c r="AV56" s="9"/>
+      <c r="AW56" s="9"/>
+      <c r="AX56" s="9"/>
+      <c r="AY56" s="9"/>
+      <c r="AZ56" s="9"/>
+      <c r="BA56" s="9"/>
+      <c r="BB56" s="9"/>
+      <c r="BC56" s="9"/>
+      <c r="BD56" s="9"/>
+      <c r="BE56" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A57" s="11"/>
+      <c r="E57" t="s">
+        <v>85</v>
+      </c>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="5"/>
+      <c r="O57" s="5"/>
+      <c r="P57" s="5"/>
+      <c r="Q57" s="5"/>
+      <c r="R57" s="5"/>
+      <c r="S57" s="5"/>
+      <c r="T57" s="5"/>
+      <c r="U57" s="5"/>
+      <c r="V57" s="5"/>
+      <c r="W57" s="5"/>
+      <c r="X57" s="5"/>
+      <c r="Y57" s="5"/>
+      <c r="Z57" s="5"/>
+      <c r="AA57" s="5"/>
+      <c r="AB57" s="5"/>
+      <c r="AC57" s="5"/>
+      <c r="AD57" s="5"/>
+      <c r="AE57" s="5"/>
+      <c r="AF57" s="5"/>
+      <c r="AG57" s="5"/>
+      <c r="AH57" s="5"/>
+      <c r="AI57" s="5"/>
+      <c r="AJ57" s="5"/>
+      <c r="AK57" s="5"/>
+      <c r="AL57" s="5"/>
+      <c r="AM57" s="5"/>
+      <c r="AN57" s="5"/>
+      <c r="AO57" s="5"/>
+      <c r="AP57" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AQ57" s="9"/>
+      <c r="AR57" s="9"/>
+      <c r="AS57" s="9"/>
+      <c r="AT57" s="9"/>
+      <c r="AU57" s="9"/>
+      <c r="AV57" s="9"/>
+      <c r="AW57" s="9"/>
+      <c r="AX57" s="9"/>
+      <c r="AY57" s="9"/>
+      <c r="AZ57" s="9"/>
+      <c r="BA57" s="9"/>
+      <c r="BB57" s="9"/>
+      <c r="BC57" s="9"/>
+      <c r="BD57" s="9"/>
+      <c r="BE57" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A58" s="11"/>
+      <c r="E58" t="s">
+        <v>84</v>
+      </c>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
+      <c r="N58" s="5"/>
+      <c r="O58" s="5"/>
+      <c r="P58" s="5"/>
+      <c r="Q58" s="5"/>
+      <c r="R58" s="5"/>
+      <c r="S58" s="5"/>
+      <c r="T58" s="5"/>
+      <c r="U58" s="5"/>
+      <c r="V58" s="5"/>
+      <c r="W58" s="5"/>
+      <c r="X58" s="5"/>
+      <c r="Y58" s="5"/>
+      <c r="Z58" s="5"/>
+      <c r="AA58" s="5"/>
+      <c r="AB58" s="5"/>
+      <c r="AC58" s="5"/>
+      <c r="AD58" s="5"/>
+      <c r="AE58" s="5"/>
+      <c r="AF58" s="5"/>
+      <c r="AG58" s="5"/>
+      <c r="AH58" s="5"/>
+      <c r="AI58" s="5"/>
+      <c r="AJ58" s="5"/>
+      <c r="AK58" s="5"/>
+      <c r="AL58" s="5"/>
+      <c r="AM58" s="5"/>
+      <c r="AN58" s="5"/>
+      <c r="AO58" s="5"/>
+      <c r="AP58" s="5"/>
+      <c r="AQ58" s="5"/>
+      <c r="AR58" s="5"/>
+      <c r="AS58" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AT58" s="9"/>
+      <c r="AU58" s="9"/>
+      <c r="AV58" s="9"/>
+      <c r="AW58" s="9"/>
+      <c r="AX58" s="9"/>
+      <c r="AY58" s="9"/>
+      <c r="AZ58" s="9"/>
+      <c r="BA58" s="9"/>
+      <c r="BB58" s="9"/>
+      <c r="BC58" s="9"/>
+      <c r="BD58" s="9"/>
+      <c r="BE58" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A59" s="11"/>
+      <c r="E59" t="s">
+        <v>86</v>
+      </c>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
+      <c r="O59" s="5"/>
+      <c r="P59" s="5"/>
+      <c r="Q59" s="5"/>
+      <c r="R59" s="5"/>
+      <c r="S59" s="5"/>
+      <c r="T59" s="5"/>
+      <c r="U59" s="5"/>
+      <c r="V59" s="5"/>
+      <c r="W59" s="5"/>
+      <c r="X59" s="5"/>
+      <c r="Y59" s="5"/>
+      <c r="Z59" s="5"/>
+      <c r="AA59" s="5"/>
+      <c r="AB59" s="5"/>
+      <c r="AC59" s="5"/>
+      <c r="AD59" s="5"/>
+      <c r="AE59" s="5"/>
+      <c r="AF59" s="5"/>
+      <c r="AG59" s="5"/>
+      <c r="AH59" s="5"/>
+      <c r="AI59" s="5"/>
+      <c r="AJ59" s="5"/>
+      <c r="AK59" s="5"/>
+      <c r="AL59" s="5"/>
+      <c r="AM59" s="5"/>
+      <c r="AN59" s="5"/>
+      <c r="AO59" s="5"/>
+      <c r="AP59" s="5"/>
+      <c r="AQ59" s="5"/>
+      <c r="AR59" s="5"/>
+      <c r="AS59" s="5"/>
+      <c r="AT59" s="5"/>
+      <c r="AU59" s="5"/>
+      <c r="AV59" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AW59" s="9"/>
+      <c r="AX59" s="9"/>
+      <c r="AY59" s="9"/>
+      <c r="AZ59" s="9"/>
+      <c r="BA59" s="9"/>
+      <c r="BB59" s="9"/>
+      <c r="BC59" s="9"/>
+      <c r="BD59" s="9"/>
+      <c r="BE59" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A60" s="11"/>
+      <c r="E60" t="s">
+        <v>87</v>
+      </c>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="5"/>
+      <c r="O60" s="5"/>
+      <c r="P60" s="5"/>
+      <c r="Q60" s="5"/>
+      <c r="R60" s="5"/>
+      <c r="S60" s="5"/>
+      <c r="T60" s="5"/>
+      <c r="U60" s="5"/>
+      <c r="V60" s="5"/>
+      <c r="W60" s="5"/>
+      <c r="X60" s="5"/>
+      <c r="Y60" s="5"/>
+      <c r="Z60" s="5"/>
+      <c r="AA60" s="5"/>
+      <c r="AB60" s="5"/>
+      <c r="AC60" s="5"/>
+      <c r="AD60" s="5"/>
+      <c r="AE60" s="5"/>
+      <c r="AF60" s="5"/>
+      <c r="AG60" s="5"/>
+      <c r="AH60" s="5"/>
+      <c r="AI60" s="5"/>
+      <c r="AJ60" s="5"/>
+      <c r="AK60" s="5"/>
+      <c r="AL60" s="5"/>
+      <c r="AM60" s="5"/>
+      <c r="AN60" s="5"/>
+      <c r="AO60" s="5"/>
+      <c r="AP60" s="5"/>
+      <c r="AQ60" s="5"/>
+      <c r="AR60" s="5"/>
+      <c r="AS60" s="5"/>
+      <c r="AT60" s="5"/>
+      <c r="AU60" s="5"/>
+      <c r="AV60" s="5"/>
+      <c r="AW60" s="5"/>
+      <c r="AX60" s="5"/>
+      <c r="AY60" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AZ60" s="9"/>
+      <c r="BA60" s="9"/>
+      <c r="BB60" s="9"/>
+      <c r="BC60" s="9"/>
+      <c r="BD60" s="9"/>
+      <c r="BE60" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>5</v>
       </c>
-      <c r="B50" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" t="s">
-        <v>30</v>
-      </c>
-      <c r="E50" t="s">
-        <v>59</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="BE61" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="62" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BE62" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BE63" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1</v>
+      </c>
+      <c r="E64" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE64" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="5:57" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>15</v>
+      </c>
+      <c r="F65" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE65" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="5:57" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>16</v>
+      </c>
+      <c r="F66" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="5:57" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>17</v>
+      </c>
+      <c r="F67" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE67" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="5:57" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
         <v>18</v>
       </c>
-      <c r="BE50" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="51" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E51" t="s">
-        <v>60</v>
-      </c>
-      <c r="K51" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE51" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="52" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>6</v>
-      </c>
-      <c r="B52" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" t="s">
-        <v>10</v>
-      </c>
-      <c r="E52" t="s">
-        <v>25</v>
-      </c>
-      <c r="F52" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE52" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="53" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E53" t="s">
-        <v>26</v>
-      </c>
-      <c r="H53" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE53" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="54" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
-        <v>27</v>
-      </c>
-      <c r="E54" t="s">
-        <v>26</v>
-      </c>
-      <c r="J54" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE54" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="55" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>16</v>
-      </c>
-      <c r="B55" t="s">
-        <v>1</v>
-      </c>
-      <c r="E55" t="s">
-        <v>17</v>
-      </c>
-      <c r="F55" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE55" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="56" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E56" t="s">
+      <c r="F68" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE68" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="69" spans="5:57" x14ac:dyDescent="0.25">
+      <c r="E69" t="s">
+        <v>31</v>
+      </c>
+      <c r="P69" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE69" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="5:57" x14ac:dyDescent="0.25">
+      <c r="E70" t="s">
+        <v>32</v>
+      </c>
+      <c r="U70" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE70" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="71" spans="5:57" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
+        <v>33</v>
+      </c>
+      <c r="U71" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE71" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="72" spans="5:57" x14ac:dyDescent="0.25">
+      <c r="E72" t="s">
+        <v>34</v>
+      </c>
+      <c r="U72" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE72" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="73" spans="5:57" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
+        <v>35</v>
+      </c>
+      <c r="U73" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE73" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="74" spans="5:57" x14ac:dyDescent="0.25">
+      <c r="E74" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z74" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE74" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="75" spans="5:57" x14ac:dyDescent="0.25">
+      <c r="E75" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z75" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE75" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="76" spans="5:57" x14ac:dyDescent="0.25">
+      <c r="E76" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE76" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE76" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="77" spans="5:57" x14ac:dyDescent="0.25">
+      <c r="E77" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ77" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE77" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="78" spans="5:57" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO78" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE78" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="79" spans="5:57" x14ac:dyDescent="0.25">
+      <c r="E79" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO79" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE79" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="80" spans="5:57" x14ac:dyDescent="0.25">
+      <c r="E80" t="s">
+        <v>41</v>
+      </c>
+      <c r="AT80" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE80" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="81" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="E81" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT81" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE81" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="82" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="E82" t="s">
+        <v>44</v>
+      </c>
+      <c r="BD82" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE82" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="83" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>21</v>
+      </c>
+      <c r="L83" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE83" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="84" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>19</v>
       </c>
-      <c r="F56" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE56" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="57" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E57" t="s">
+      <c r="E84" t="s">
         <v>20</v>
       </c>
-      <c r="F57" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE57" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="58" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E58" t="s">
-        <v>21</v>
-      </c>
-      <c r="F58" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE58" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="59" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E59" t="s">
-        <v>22</v>
-      </c>
-      <c r="F59" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE59" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="60" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E60" t="s">
-        <v>40</v>
-      </c>
-      <c r="P60" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE60" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="61" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E61" t="s">
-        <v>41</v>
-      </c>
-      <c r="U61" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE61" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="62" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E62" t="s">
-        <v>42</v>
-      </c>
-      <c r="U62" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE62" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="63" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E63" t="s">
-        <v>43</v>
-      </c>
-      <c r="U63" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE63" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="64" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E64" t="s">
-        <v>44</v>
-      </c>
-      <c r="U64" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE64" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="65" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E65" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z65" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE65" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="66" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E66" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z66" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE66" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="67" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E67" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE67" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE67" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="68" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E68" t="s">
-        <v>48</v>
-      </c>
-      <c r="AJ68" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE68" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="69" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E69" t="s">
-        <v>49</v>
-      </c>
-      <c r="AO69" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE69" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="70" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E70" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO70" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE70" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="71" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E71" t="s">
-        <v>50</v>
-      </c>
-      <c r="AT71" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE71" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="72" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E72" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT72" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE72" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="73" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E73" t="s">
-        <v>53</v>
-      </c>
-      <c r="BD73" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE73" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="74" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>28</v>
-      </c>
-      <c r="C74" t="s">
-        <v>8</v>
-      </c>
-      <c r="E74" t="s">
-        <v>29</v>
-      </c>
-      <c r="L74" t="s">
-        <v>18</v>
-      </c>
-      <c r="BE74" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="75" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>23</v>
-      </c>
-      <c r="E75" t="s">
-        <v>24</v>
-      </c>
-      <c r="F75" t="s">
-        <v>18</v>
+      <c r="F84" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="D1:D2"/>
     <mergeCell ref="A34:A49"/>
-    <mergeCell ref="D1:D2"/>
     <mergeCell ref="F1:BD1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>

</xml_diff>

<commit_message>
Additional speeds added for hosting.
</commit_message>
<xml_diff>
--- a/ReleaseTimelines.xlsx
+++ b/ReleaseTimelines.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="95">
   <si>
     <t>Dev</t>
   </si>
@@ -251,21 +251,6 @@
     <t>Remote Support</t>
   </si>
   <si>
-    <t>ARPANET 50 Kbps</t>
-  </si>
-  <si>
-    <t>NSFNET 56 Kbps</t>
-  </si>
-  <si>
-    <t>NSFNET 45 Mbps</t>
-  </si>
-  <si>
-    <t>NSFNET 145 Mbps</t>
-  </si>
-  <si>
-    <t>Specialist</t>
-  </si>
-  <si>
     <t>Dial-up 56 Kbps</t>
   </si>
   <si>
@@ -288,6 +273,42 @@
   </si>
   <si>
     <t>Fibre 1 Gbps</t>
+  </si>
+  <si>
+    <t>T1 1.5 Mbps</t>
+  </si>
+  <si>
+    <t>T3 45 Mbps</t>
+  </si>
+  <si>
+    <t>OC-3 155 Mbps</t>
+  </si>
+  <si>
+    <t>OC-12 622 Mbps</t>
+  </si>
+  <si>
+    <t>OC-1 51 Mbps</t>
+  </si>
+  <si>
+    <t>OC-48 2.4 Gbps</t>
+  </si>
+  <si>
+    <t>OC-192 9.6 Gbps</t>
+  </si>
+  <si>
+    <t>OC-256 13.1 Gbps</t>
+  </si>
+  <si>
+    <t>OC-768 40 Gbps</t>
+  </si>
+  <si>
+    <t>T1C 3.2 Mbps</t>
+  </si>
+  <si>
+    <t>T2 6.3 Mbps</t>
+  </si>
+  <si>
+    <t>T4 274 Mbps</t>
   </si>
 </sst>
 </file>
@@ -685,13 +706,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE84"/>
+  <dimension ref="A1:BE92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="AD24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C54" sqref="C54"/>
+      <selection pane="bottomRight" activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2853,12 +2874,14 @@
         <v>34</v>
       </c>
       <c r="C50" t="s">
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="E50" t="s">
-        <v>75</v>
-      </c>
-      <c r="F50" s="5"/>
+        <v>83</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
@@ -2918,7 +2941,7 @@
     <row r="51" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="E51" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
@@ -2936,11 +2959,11 @@
       <c r="S51" s="5"/>
       <c r="T51" s="5"/>
       <c r="U51" s="5"/>
-      <c r="V51" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="W51" s="12"/>
-      <c r="X51" s="12"/>
+      <c r="V51" s="5"/>
+      <c r="W51" s="5"/>
+      <c r="X51" s="12" t="s">
+        <v>14</v>
+      </c>
       <c r="Y51" s="12"/>
       <c r="Z51" s="12"/>
       <c r="AA51" s="12"/>
@@ -2980,7 +3003,7 @@
     <row r="52" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="E52" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
@@ -3000,12 +3023,10 @@
       <c r="U52" s="5"/>
       <c r="V52" s="5"/>
       <c r="W52" s="5"/>
-      <c r="X52" s="5"/>
-      <c r="Y52" s="5"/>
-      <c r="Z52" s="5"/>
-      <c r="AA52" s="12" t="s">
-        <v>14</v>
-      </c>
+      <c r="X52" s="12"/>
+      <c r="Y52" s="12"/>
+      <c r="Z52" s="12"/>
+      <c r="AA52" s="12"/>
       <c r="AB52" s="12"/>
       <c r="AC52" s="12"/>
       <c r="AD52" s="12"/>
@@ -3035,14 +3056,12 @@
       <c r="BB52" s="12"/>
       <c r="BC52" s="12"/>
       <c r="BD52" s="12"/>
-      <c r="BE52" s="12" t="s">
-        <v>65</v>
-      </c>
+      <c r="BE52" s="12"/>
     </row>
     <row r="53" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A53" s="11"/>
       <c r="E53" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
@@ -3062,15 +3081,13 @@
       <c r="U53" s="5"/>
       <c r="V53" s="5"/>
       <c r="W53" s="5"/>
-      <c r="X53" s="5"/>
-      <c r="Y53" s="5"/>
-      <c r="Z53" s="5"/>
-      <c r="AA53" s="5"/>
-      <c r="AB53" s="5"/>
-      <c r="AC53" s="5"/>
-      <c r="AD53" s="12" t="s">
-        <v>14</v>
-      </c>
+      <c r="X53" s="12"/>
+      <c r="Y53" s="12"/>
+      <c r="Z53" s="12"/>
+      <c r="AA53" s="12"/>
+      <c r="AB53" s="12"/>
+      <c r="AC53" s="12"/>
+      <c r="AD53" s="12"/>
       <c r="AE53" s="12"/>
       <c r="AF53" s="12"/>
       <c r="AG53" s="12"/>
@@ -3097,17 +3114,12 @@
       <c r="BB53" s="12"/>
       <c r="BC53" s="12"/>
       <c r="BD53" s="12"/>
-      <c r="BE53" s="12" t="s">
-        <v>65</v>
-      </c>
+      <c r="BE53" s="12"/>
     </row>
     <row r="54" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
-      <c r="C54" t="s">
-        <v>81</v>
-      </c>
       <c r="E54" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
@@ -3131,45 +3143,45 @@
       <c r="Y54" s="5"/>
       <c r="Z54" s="5"/>
       <c r="AA54" s="5"/>
-      <c r="AB54" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC54" s="9"/>
-      <c r="AD54" s="9"/>
-      <c r="AE54" s="9"/>
-      <c r="AF54" s="9"/>
-      <c r="AG54" s="9"/>
-      <c r="AH54" s="9"/>
-      <c r="AI54" s="9"/>
-      <c r="AJ54" s="9"/>
-      <c r="AK54" s="9"/>
-      <c r="AL54" s="9"/>
-      <c r="AM54" s="9"/>
-      <c r="AN54" s="9"/>
-      <c r="AO54" s="9"/>
-      <c r="AP54" s="9"/>
-      <c r="AQ54" s="9"/>
-      <c r="AR54" s="9"/>
-      <c r="AS54" s="9"/>
-      <c r="AT54" s="9"/>
-      <c r="AU54" s="9"/>
-      <c r="AV54" s="9"/>
-      <c r="AW54" s="9"/>
-      <c r="AX54" s="9"/>
-      <c r="AY54" s="9"/>
-      <c r="AZ54" s="9"/>
-      <c r="BA54" s="9"/>
-      <c r="BB54" s="9"/>
-      <c r="BC54" s="9"/>
-      <c r="BD54" s="9"/>
-      <c r="BE54" s="9" t="s">
+      <c r="AB54" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC54" s="12"/>
+      <c r="AD54" s="12"/>
+      <c r="AE54" s="12"/>
+      <c r="AF54" s="12"/>
+      <c r="AG54" s="12"/>
+      <c r="AH54" s="12"/>
+      <c r="AI54" s="12"/>
+      <c r="AJ54" s="12"/>
+      <c r="AK54" s="12"/>
+      <c r="AL54" s="12"/>
+      <c r="AM54" s="12"/>
+      <c r="AN54" s="12"/>
+      <c r="AO54" s="12"/>
+      <c r="AP54" s="12"/>
+      <c r="AQ54" s="12"/>
+      <c r="AR54" s="12"/>
+      <c r="AS54" s="12"/>
+      <c r="AT54" s="12"/>
+      <c r="AU54" s="12"/>
+      <c r="AV54" s="12"/>
+      <c r="AW54" s="12"/>
+      <c r="AX54" s="12"/>
+      <c r="AY54" s="12"/>
+      <c r="AZ54" s="12"/>
+      <c r="BA54" s="12"/>
+      <c r="BB54" s="12"/>
+      <c r="BC54" s="12"/>
+      <c r="BD54" s="12"/>
+      <c r="BE54" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A55" s="11"/>
       <c r="E55" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
@@ -3193,45 +3205,41 @@
       <c r="Y55" s="5"/>
       <c r="Z55" s="5"/>
       <c r="AA55" s="5"/>
-      <c r="AB55" s="5"/>
-      <c r="AC55" s="5"/>
-      <c r="AD55" s="5"/>
-      <c r="AE55" s="5"/>
-      <c r="AF55" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG55" s="9"/>
-      <c r="AH55" s="9"/>
-      <c r="AI55" s="9"/>
-      <c r="AJ55" s="9"/>
-      <c r="AK55" s="9"/>
-      <c r="AL55" s="9"/>
-      <c r="AM55" s="9"/>
-      <c r="AN55" s="9"/>
-      <c r="AO55" s="9"/>
-      <c r="AP55" s="9"/>
-      <c r="AQ55" s="9"/>
-      <c r="AR55" s="9"/>
-      <c r="AS55" s="9"/>
-      <c r="AT55" s="9"/>
-      <c r="AU55" s="9"/>
-      <c r="AV55" s="9"/>
-      <c r="AW55" s="9"/>
-      <c r="AX55" s="9"/>
-      <c r="AY55" s="9"/>
-      <c r="AZ55" s="9"/>
-      <c r="BA55" s="9"/>
-      <c r="BB55" s="9"/>
-      <c r="BC55" s="9"/>
-      <c r="BD55" s="9"/>
-      <c r="BE55" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB55" s="12"/>
+      <c r="AC55" s="12"/>
+      <c r="AD55" s="12"/>
+      <c r="AE55" s="12"/>
+      <c r="AF55" s="12"/>
+      <c r="AG55" s="12"/>
+      <c r="AH55" s="12"/>
+      <c r="AI55" s="12"/>
+      <c r="AJ55" s="12"/>
+      <c r="AK55" s="12"/>
+      <c r="AL55" s="12"/>
+      <c r="AM55" s="12"/>
+      <c r="AN55" s="12"/>
+      <c r="AO55" s="12"/>
+      <c r="AP55" s="12"/>
+      <c r="AQ55" s="12"/>
+      <c r="AR55" s="12"/>
+      <c r="AS55" s="12"/>
+      <c r="AT55" s="12"/>
+      <c r="AU55" s="12"/>
+      <c r="AV55" s="12"/>
+      <c r="AW55" s="12"/>
+      <c r="AX55" s="12"/>
+      <c r="AY55" s="12"/>
+      <c r="AZ55" s="12"/>
+      <c r="BA55" s="12"/>
+      <c r="BB55" s="12"/>
+      <c r="BC55" s="12"/>
+      <c r="BD55" s="12"/>
+      <c r="BE55" s="12"/>
     </row>
     <row r="56" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A56" s="11"/>
       <c r="E56" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
@@ -3255,45 +3263,41 @@
       <c r="Y56" s="5"/>
       <c r="Z56" s="5"/>
       <c r="AA56" s="5"/>
-      <c r="AB56" s="5"/>
-      <c r="AC56" s="5"/>
-      <c r="AD56" s="5"/>
-      <c r="AE56" s="5"/>
-      <c r="AF56" s="5"/>
-      <c r="AG56" s="5"/>
-      <c r="AH56" s="5"/>
-      <c r="AI56" s="5"/>
-      <c r="AJ56" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AK56" s="9"/>
-      <c r="AL56" s="9"/>
-      <c r="AM56" s="9"/>
-      <c r="AN56" s="9"/>
-      <c r="AO56" s="9"/>
-      <c r="AP56" s="9"/>
-      <c r="AQ56" s="9"/>
-      <c r="AR56" s="9"/>
-      <c r="AS56" s="9"/>
-      <c r="AT56" s="9"/>
-      <c r="AU56" s="9"/>
-      <c r="AV56" s="9"/>
-      <c r="AW56" s="9"/>
-      <c r="AX56" s="9"/>
-      <c r="AY56" s="9"/>
-      <c r="AZ56" s="9"/>
-      <c r="BA56" s="9"/>
-      <c r="BB56" s="9"/>
-      <c r="BC56" s="9"/>
-      <c r="BD56" s="9"/>
-      <c r="BE56" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB56" s="12"/>
+      <c r="AC56" s="12"/>
+      <c r="AD56" s="12"/>
+      <c r="AE56" s="12"/>
+      <c r="AF56" s="12"/>
+      <c r="AG56" s="12"/>
+      <c r="AH56" s="12"/>
+      <c r="AI56" s="12"/>
+      <c r="AJ56" s="12"/>
+      <c r="AK56" s="12"/>
+      <c r="AL56" s="12"/>
+      <c r="AM56" s="12"/>
+      <c r="AN56" s="12"/>
+      <c r="AO56" s="12"/>
+      <c r="AP56" s="12"/>
+      <c r="AQ56" s="12"/>
+      <c r="AR56" s="12"/>
+      <c r="AS56" s="12"/>
+      <c r="AT56" s="12"/>
+      <c r="AU56" s="12"/>
+      <c r="AV56" s="12"/>
+      <c r="AW56" s="12"/>
+      <c r="AX56" s="12"/>
+      <c r="AY56" s="12"/>
+      <c r="AZ56" s="12"/>
+      <c r="BA56" s="12"/>
+      <c r="BB56" s="12"/>
+      <c r="BC56" s="12"/>
+      <c r="BD56" s="12"/>
+      <c r="BE56" s="12"/>
     </row>
     <row r="57" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A57" s="11"/>
       <c r="E57" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
@@ -3317,45 +3321,41 @@
       <c r="Y57" s="5"/>
       <c r="Z57" s="5"/>
       <c r="AA57" s="5"/>
-      <c r="AB57" s="5"/>
-      <c r="AC57" s="5"/>
-      <c r="AD57" s="5"/>
-      <c r="AE57" s="5"/>
-      <c r="AF57" s="5"/>
-      <c r="AG57" s="5"/>
-      <c r="AH57" s="5"/>
-      <c r="AI57" s="5"/>
-      <c r="AJ57" s="5"/>
-      <c r="AK57" s="5"/>
-      <c r="AL57" s="5"/>
-      <c r="AM57" s="5"/>
-      <c r="AN57" s="5"/>
-      <c r="AO57" s="5"/>
-      <c r="AP57" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AQ57" s="9"/>
-      <c r="AR57" s="9"/>
-      <c r="AS57" s="9"/>
-      <c r="AT57" s="9"/>
-      <c r="AU57" s="9"/>
-      <c r="AV57" s="9"/>
-      <c r="AW57" s="9"/>
-      <c r="AX57" s="9"/>
-      <c r="AY57" s="9"/>
-      <c r="AZ57" s="9"/>
-      <c r="BA57" s="9"/>
-      <c r="BB57" s="9"/>
-      <c r="BC57" s="9"/>
-      <c r="BD57" s="9"/>
-      <c r="BE57" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB57" s="12"/>
+      <c r="AC57" s="12"/>
+      <c r="AD57" s="12"/>
+      <c r="AE57" s="12"/>
+      <c r="AF57" s="12"/>
+      <c r="AG57" s="12"/>
+      <c r="AH57" s="12"/>
+      <c r="AI57" s="12"/>
+      <c r="AJ57" s="12"/>
+      <c r="AK57" s="12"/>
+      <c r="AL57" s="12"/>
+      <c r="AM57" s="12"/>
+      <c r="AN57" s="12"/>
+      <c r="AO57" s="12"/>
+      <c r="AP57" s="12"/>
+      <c r="AQ57" s="12"/>
+      <c r="AR57" s="12"/>
+      <c r="AS57" s="12"/>
+      <c r="AT57" s="12"/>
+      <c r="AU57" s="12"/>
+      <c r="AV57" s="12"/>
+      <c r="AW57" s="12"/>
+      <c r="AX57" s="12"/>
+      <c r="AY57" s="12"/>
+      <c r="AZ57" s="12"/>
+      <c r="BA57" s="12"/>
+      <c r="BB57" s="12"/>
+      <c r="BC57" s="12"/>
+      <c r="BD57" s="12"/>
+      <c r="BE57" s="12"/>
     </row>
     <row r="58" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
       <c r="E58" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
@@ -3379,45 +3379,41 @@
       <c r="Y58" s="5"/>
       <c r="Z58" s="5"/>
       <c r="AA58" s="5"/>
-      <c r="AB58" s="5"/>
-      <c r="AC58" s="5"/>
-      <c r="AD58" s="5"/>
-      <c r="AE58" s="5"/>
-      <c r="AF58" s="5"/>
-      <c r="AG58" s="5"/>
-      <c r="AH58" s="5"/>
-      <c r="AI58" s="5"/>
-      <c r="AJ58" s="5"/>
-      <c r="AK58" s="5"/>
-      <c r="AL58" s="5"/>
-      <c r="AM58" s="5"/>
-      <c r="AN58" s="5"/>
-      <c r="AO58" s="5"/>
-      <c r="AP58" s="5"/>
-      <c r="AQ58" s="5"/>
-      <c r="AR58" s="5"/>
-      <c r="AS58" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AT58" s="9"/>
-      <c r="AU58" s="9"/>
-      <c r="AV58" s="9"/>
-      <c r="AW58" s="9"/>
-      <c r="AX58" s="9"/>
-      <c r="AY58" s="9"/>
-      <c r="AZ58" s="9"/>
-      <c r="BA58" s="9"/>
-      <c r="BB58" s="9"/>
-      <c r="BC58" s="9"/>
-      <c r="BD58" s="9"/>
-      <c r="BE58" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB58" s="12"/>
+      <c r="AC58" s="12"/>
+      <c r="AD58" s="12"/>
+      <c r="AE58" s="12"/>
+      <c r="AF58" s="12"/>
+      <c r="AG58" s="12"/>
+      <c r="AH58" s="12"/>
+      <c r="AI58" s="12"/>
+      <c r="AJ58" s="12"/>
+      <c r="AK58" s="12"/>
+      <c r="AL58" s="12"/>
+      <c r="AM58" s="12"/>
+      <c r="AN58" s="12"/>
+      <c r="AO58" s="12"/>
+      <c r="AP58" s="12"/>
+      <c r="AQ58" s="12"/>
+      <c r="AR58" s="12"/>
+      <c r="AS58" s="12"/>
+      <c r="AT58" s="12"/>
+      <c r="AU58" s="12"/>
+      <c r="AV58" s="12"/>
+      <c r="AW58" s="12"/>
+      <c r="AX58" s="12"/>
+      <c r="AY58" s="12"/>
+      <c r="AZ58" s="12"/>
+      <c r="BA58" s="12"/>
+      <c r="BB58" s="12"/>
+      <c r="BC58" s="12"/>
+      <c r="BD58" s="12"/>
+      <c r="BE58" s="12"/>
     </row>
     <row r="59" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
       <c r="E59" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
@@ -3441,45 +3437,41 @@
       <c r="Y59" s="5"/>
       <c r="Z59" s="5"/>
       <c r="AA59" s="5"/>
-      <c r="AB59" s="5"/>
-      <c r="AC59" s="5"/>
-      <c r="AD59" s="5"/>
-      <c r="AE59" s="5"/>
-      <c r="AF59" s="5"/>
-      <c r="AG59" s="5"/>
-      <c r="AH59" s="5"/>
-      <c r="AI59" s="5"/>
-      <c r="AJ59" s="5"/>
-      <c r="AK59" s="5"/>
-      <c r="AL59" s="5"/>
-      <c r="AM59" s="5"/>
-      <c r="AN59" s="5"/>
-      <c r="AO59" s="5"/>
-      <c r="AP59" s="5"/>
-      <c r="AQ59" s="5"/>
-      <c r="AR59" s="5"/>
-      <c r="AS59" s="5"/>
-      <c r="AT59" s="5"/>
-      <c r="AU59" s="5"/>
-      <c r="AV59" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AW59" s="9"/>
-      <c r="AX59" s="9"/>
-      <c r="AY59" s="9"/>
-      <c r="AZ59" s="9"/>
-      <c r="BA59" s="9"/>
-      <c r="BB59" s="9"/>
-      <c r="BC59" s="9"/>
-      <c r="BD59" s="9"/>
-      <c r="BE59" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB59" s="12"/>
+      <c r="AC59" s="12"/>
+      <c r="AD59" s="12"/>
+      <c r="AE59" s="12"/>
+      <c r="AF59" s="12"/>
+      <c r="AG59" s="12"/>
+      <c r="AH59" s="12"/>
+      <c r="AI59" s="12"/>
+      <c r="AJ59" s="12"/>
+      <c r="AK59" s="12"/>
+      <c r="AL59" s="12"/>
+      <c r="AM59" s="12"/>
+      <c r="AN59" s="12"/>
+      <c r="AO59" s="12"/>
+      <c r="AP59" s="12"/>
+      <c r="AQ59" s="12"/>
+      <c r="AR59" s="12"/>
+      <c r="AS59" s="12"/>
+      <c r="AT59" s="12"/>
+      <c r="AU59" s="12"/>
+      <c r="AV59" s="12"/>
+      <c r="AW59" s="12"/>
+      <c r="AX59" s="12"/>
+      <c r="AY59" s="12"/>
+      <c r="AZ59" s="12"/>
+      <c r="BA59" s="12"/>
+      <c r="BB59" s="12"/>
+      <c r="BC59" s="12"/>
+      <c r="BD59" s="12"/>
+      <c r="BE59" s="12"/>
     </row>
     <row r="60" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A60" s="11"/>
       <c r="E60" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
@@ -3503,246 +3495,649 @@
       <c r="Y60" s="5"/>
       <c r="Z60" s="5"/>
       <c r="AA60" s="5"/>
-      <c r="AB60" s="5"/>
-      <c r="AC60" s="5"/>
-      <c r="AD60" s="5"/>
-      <c r="AE60" s="5"/>
-      <c r="AF60" s="5"/>
-      <c r="AG60" s="5"/>
-      <c r="AH60" s="5"/>
-      <c r="AI60" s="5"/>
-      <c r="AJ60" s="5"/>
-      <c r="AK60" s="5"/>
-      <c r="AL60" s="5"/>
-      <c r="AM60" s="5"/>
-      <c r="AN60" s="5"/>
-      <c r="AO60" s="5"/>
-      <c r="AP60" s="5"/>
-      <c r="AQ60" s="5"/>
-      <c r="AR60" s="5"/>
-      <c r="AS60" s="5"/>
-      <c r="AT60" s="5"/>
-      <c r="AU60" s="5"/>
-      <c r="AV60" s="5"/>
-      <c r="AW60" s="5"/>
-      <c r="AX60" s="5"/>
-      <c r="AY60" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AZ60" s="9"/>
-      <c r="BA60" s="9"/>
-      <c r="BB60" s="9"/>
-      <c r="BC60" s="9"/>
-      <c r="BD60" s="9"/>
-      <c r="BE60" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="AB60" s="12"/>
+      <c r="AC60" s="12"/>
+      <c r="AD60" s="12"/>
+      <c r="AE60" s="12"/>
+      <c r="AF60" s="12"/>
+      <c r="AG60" s="12"/>
+      <c r="AH60" s="12"/>
+      <c r="AI60" s="12"/>
+      <c r="AJ60" s="12"/>
+      <c r="AK60" s="12"/>
+      <c r="AL60" s="12"/>
+      <c r="AM60" s="12"/>
+      <c r="AN60" s="12"/>
+      <c r="AO60" s="12"/>
+      <c r="AP60" s="12"/>
+      <c r="AQ60" s="12"/>
+      <c r="AR60" s="12"/>
+      <c r="AS60" s="12"/>
+      <c r="AT60" s="12"/>
+      <c r="AU60" s="12"/>
+      <c r="AV60" s="12"/>
+      <c r="AW60" s="12"/>
+      <c r="AX60" s="12"/>
+      <c r="AY60" s="12"/>
+      <c r="AZ60" s="12"/>
+      <c r="BA60" s="12"/>
+      <c r="BB60" s="12"/>
+      <c r="BC60" s="12"/>
+      <c r="BD60" s="12"/>
+      <c r="BE60" s="12"/>
     </row>
     <row r="61" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="A61" s="11"/>
+      <c r="E61" t="s">
+        <v>91</v>
+      </c>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
+      <c r="N61" s="5"/>
+      <c r="O61" s="5"/>
+      <c r="P61" s="5"/>
+      <c r="Q61" s="5"/>
+      <c r="R61" s="5"/>
+      <c r="S61" s="5"/>
+      <c r="T61" s="5"/>
+      <c r="U61" s="5"/>
+      <c r="V61" s="5"/>
+      <c r="W61" s="5"/>
+      <c r="X61" s="5"/>
+      <c r="Y61" s="5"/>
+      <c r="Z61" s="5"/>
+      <c r="AA61" s="5"/>
+      <c r="AB61" s="12"/>
+      <c r="AC61" s="12"/>
+      <c r="AD61" s="12"/>
+      <c r="AE61" s="12"/>
+      <c r="AF61" s="12"/>
+      <c r="AG61" s="12"/>
+      <c r="AH61" s="12"/>
+      <c r="AI61" s="12"/>
+      <c r="AJ61" s="12"/>
+      <c r="AK61" s="12"/>
+      <c r="AL61" s="12"/>
+      <c r="AM61" s="12"/>
+      <c r="AN61" s="12"/>
+      <c r="AO61" s="12"/>
+      <c r="AP61" s="12"/>
+      <c r="AQ61" s="12"/>
+      <c r="AR61" s="12"/>
+      <c r="AS61" s="12"/>
+      <c r="AT61" s="12"/>
+      <c r="AU61" s="12"/>
+      <c r="AV61" s="12"/>
+      <c r="AW61" s="12"/>
+      <c r="AX61" s="12"/>
+      <c r="AY61" s="12"/>
+      <c r="AZ61" s="12"/>
+      <c r="BA61" s="12"/>
+      <c r="BB61" s="12"/>
+      <c r="BC61" s="12"/>
+      <c r="BD61" s="12"/>
+      <c r="BE61" s="12"/>
+    </row>
+    <row r="62" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A62" s="11"/>
+      <c r="C62" t="s">
+        <v>76</v>
+      </c>
+      <c r="E62" t="s">
+        <v>75</v>
+      </c>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="5"/>
+      <c r="O62" s="5"/>
+      <c r="P62" s="5"/>
+      <c r="Q62" s="5"/>
+      <c r="R62" s="5"/>
+      <c r="S62" s="5"/>
+      <c r="T62" s="5"/>
+      <c r="U62" s="5"/>
+      <c r="V62" s="5"/>
+      <c r="W62" s="5"/>
+      <c r="X62" s="5"/>
+      <c r="Y62" s="5"/>
+      <c r="Z62" s="5"/>
+      <c r="AA62" s="5"/>
+      <c r="AB62" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC62" s="9"/>
+      <c r="AD62" s="9"/>
+      <c r="AE62" s="9"/>
+      <c r="AF62" s="9"/>
+      <c r="AG62" s="9"/>
+      <c r="AH62" s="9"/>
+      <c r="AI62" s="9"/>
+      <c r="AJ62" s="9"/>
+      <c r="AK62" s="9"/>
+      <c r="AL62" s="9"/>
+      <c r="AM62" s="9"/>
+      <c r="AN62" s="9"/>
+      <c r="AO62" s="9"/>
+      <c r="AP62" s="9"/>
+      <c r="AQ62" s="9"/>
+      <c r="AR62" s="9"/>
+      <c r="AS62" s="9"/>
+      <c r="AT62" s="9"/>
+      <c r="AU62" s="9"/>
+      <c r="AV62" s="9"/>
+      <c r="AW62" s="9"/>
+      <c r="AX62" s="9"/>
+      <c r="AY62" s="9"/>
+      <c r="AZ62" s="9"/>
+      <c r="BA62" s="9"/>
+      <c r="BB62" s="9"/>
+      <c r="BC62" s="9"/>
+      <c r="BD62" s="9"/>
+      <c r="BE62" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A63" s="11"/>
+      <c r="E63" t="s">
+        <v>78</v>
+      </c>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="5"/>
+      <c r="O63" s="5"/>
+      <c r="P63" s="5"/>
+      <c r="Q63" s="5"/>
+      <c r="R63" s="5"/>
+      <c r="S63" s="5"/>
+      <c r="T63" s="5"/>
+      <c r="U63" s="5"/>
+      <c r="V63" s="5"/>
+      <c r="W63" s="5"/>
+      <c r="X63" s="5"/>
+      <c r="Y63" s="5"/>
+      <c r="Z63" s="5"/>
+      <c r="AA63" s="5"/>
+      <c r="AB63" s="5"/>
+      <c r="AC63" s="5"/>
+      <c r="AD63" s="5"/>
+      <c r="AE63" s="5"/>
+      <c r="AF63" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG63" s="9"/>
+      <c r="AH63" s="9"/>
+      <c r="AI63" s="9"/>
+      <c r="AJ63" s="9"/>
+      <c r="AK63" s="9"/>
+      <c r="AL63" s="9"/>
+      <c r="AM63" s="9"/>
+      <c r="AN63" s="9"/>
+      <c r="AO63" s="9"/>
+      <c r="AP63" s="9"/>
+      <c r="AQ63" s="9"/>
+      <c r="AR63" s="9"/>
+      <c r="AS63" s="9"/>
+      <c r="AT63" s="9"/>
+      <c r="AU63" s="9"/>
+      <c r="AV63" s="9"/>
+      <c r="AW63" s="9"/>
+      <c r="AX63" s="9"/>
+      <c r="AY63" s="9"/>
+      <c r="AZ63" s="9"/>
+      <c r="BA63" s="9"/>
+      <c r="BB63" s="9"/>
+      <c r="BC63" s="9"/>
+      <c r="BD63" s="9"/>
+      <c r="BE63" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A64" s="11"/>
+      <c r="E64" t="s">
+        <v>77</v>
+      </c>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
+      <c r="K64" s="5"/>
+      <c r="L64" s="5"/>
+      <c r="M64" s="5"/>
+      <c r="N64" s="5"/>
+      <c r="O64" s="5"/>
+      <c r="P64" s="5"/>
+      <c r="Q64" s="5"/>
+      <c r="R64" s="5"/>
+      <c r="S64" s="5"/>
+      <c r="T64" s="5"/>
+      <c r="U64" s="5"/>
+      <c r="V64" s="5"/>
+      <c r="W64" s="5"/>
+      <c r="X64" s="5"/>
+      <c r="Y64" s="5"/>
+      <c r="Z64" s="5"/>
+      <c r="AA64" s="5"/>
+      <c r="AB64" s="5"/>
+      <c r="AC64" s="5"/>
+      <c r="AD64" s="5"/>
+      <c r="AE64" s="5"/>
+      <c r="AF64" s="5"/>
+      <c r="AG64" s="5"/>
+      <c r="AH64" s="5"/>
+      <c r="AI64" s="5"/>
+      <c r="AJ64" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK64" s="9"/>
+      <c r="AL64" s="9"/>
+      <c r="AM64" s="9"/>
+      <c r="AN64" s="9"/>
+      <c r="AO64" s="9"/>
+      <c r="AP64" s="9"/>
+      <c r="AQ64" s="9"/>
+      <c r="AR64" s="9"/>
+      <c r="AS64" s="9"/>
+      <c r="AT64" s="9"/>
+      <c r="AU64" s="9"/>
+      <c r="AV64" s="9"/>
+      <c r="AW64" s="9"/>
+      <c r="AX64" s="9"/>
+      <c r="AY64" s="9"/>
+      <c r="AZ64" s="9"/>
+      <c r="BA64" s="9"/>
+      <c r="BB64" s="9"/>
+      <c r="BC64" s="9"/>
+      <c r="BD64" s="9"/>
+      <c r="BE64" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A65" s="11"/>
+      <c r="E65" t="s">
+        <v>80</v>
+      </c>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5"/>
+      <c r="K65" s="5"/>
+      <c r="L65" s="5"/>
+      <c r="M65" s="5"/>
+      <c r="N65" s="5"/>
+      <c r="O65" s="5"/>
+      <c r="P65" s="5"/>
+      <c r="Q65" s="5"/>
+      <c r="R65" s="5"/>
+      <c r="S65" s="5"/>
+      <c r="T65" s="5"/>
+      <c r="U65" s="5"/>
+      <c r="V65" s="5"/>
+      <c r="W65" s="5"/>
+      <c r="X65" s="5"/>
+      <c r="Y65" s="5"/>
+      <c r="Z65" s="5"/>
+      <c r="AA65" s="5"/>
+      <c r="AB65" s="5"/>
+      <c r="AC65" s="5"/>
+      <c r="AD65" s="5"/>
+      <c r="AE65" s="5"/>
+      <c r="AF65" s="5"/>
+      <c r="AG65" s="5"/>
+      <c r="AH65" s="5"/>
+      <c r="AI65" s="5"/>
+      <c r="AJ65" s="5"/>
+      <c r="AK65" s="5"/>
+      <c r="AL65" s="5"/>
+      <c r="AM65" s="5"/>
+      <c r="AN65" s="5"/>
+      <c r="AO65" s="5"/>
+      <c r="AP65" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AQ65" s="9"/>
+      <c r="AR65" s="9"/>
+      <c r="AS65" s="9"/>
+      <c r="AT65" s="9"/>
+      <c r="AU65" s="9"/>
+      <c r="AV65" s="9"/>
+      <c r="AW65" s="9"/>
+      <c r="AX65" s="9"/>
+      <c r="AY65" s="9"/>
+      <c r="AZ65" s="9"/>
+      <c r="BA65" s="9"/>
+      <c r="BB65" s="9"/>
+      <c r="BC65" s="9"/>
+      <c r="BD65" s="9"/>
+      <c r="BE65" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A66" s="11"/>
+      <c r="E66" t="s">
+        <v>79</v>
+      </c>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="5"/>
+      <c r="O66" s="5"/>
+      <c r="P66" s="5"/>
+      <c r="Q66" s="5"/>
+      <c r="R66" s="5"/>
+      <c r="S66" s="5"/>
+      <c r="T66" s="5"/>
+      <c r="U66" s="5"/>
+      <c r="V66" s="5"/>
+      <c r="W66" s="5"/>
+      <c r="X66" s="5"/>
+      <c r="Y66" s="5"/>
+      <c r="Z66" s="5"/>
+      <c r="AA66" s="5"/>
+      <c r="AB66" s="5"/>
+      <c r="AC66" s="5"/>
+      <c r="AD66" s="5"/>
+      <c r="AE66" s="5"/>
+      <c r="AF66" s="5"/>
+      <c r="AG66" s="5"/>
+      <c r="AH66" s="5"/>
+      <c r="AI66" s="5"/>
+      <c r="AJ66" s="5"/>
+      <c r="AK66" s="5"/>
+      <c r="AL66" s="5"/>
+      <c r="AM66" s="5"/>
+      <c r="AN66" s="5"/>
+      <c r="AO66" s="5"/>
+      <c r="AP66" s="5"/>
+      <c r="AQ66" s="5"/>
+      <c r="AR66" s="5"/>
+      <c r="AS66" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AT66" s="9"/>
+      <c r="AU66" s="9"/>
+      <c r="AV66" s="9"/>
+      <c r="AW66" s="9"/>
+      <c r="AX66" s="9"/>
+      <c r="AY66" s="9"/>
+      <c r="AZ66" s="9"/>
+      <c r="BA66" s="9"/>
+      <c r="BB66" s="9"/>
+      <c r="BC66" s="9"/>
+      <c r="BD66" s="9"/>
+      <c r="BE66" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A67" s="11"/>
+      <c r="E67" t="s">
+        <v>81</v>
+      </c>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5"/>
+      <c r="O67" s="5"/>
+      <c r="P67" s="5"/>
+      <c r="Q67" s="5"/>
+      <c r="R67" s="5"/>
+      <c r="S67" s="5"/>
+      <c r="T67" s="5"/>
+      <c r="U67" s="5"/>
+      <c r="V67" s="5"/>
+      <c r="W67" s="5"/>
+      <c r="X67" s="5"/>
+      <c r="Y67" s="5"/>
+      <c r="Z67" s="5"/>
+      <c r="AA67" s="5"/>
+      <c r="AB67" s="5"/>
+      <c r="AC67" s="5"/>
+      <c r="AD67" s="5"/>
+      <c r="AE67" s="5"/>
+      <c r="AF67" s="5"/>
+      <c r="AG67" s="5"/>
+      <c r="AH67" s="5"/>
+      <c r="AI67" s="5"/>
+      <c r="AJ67" s="5"/>
+      <c r="AK67" s="5"/>
+      <c r="AL67" s="5"/>
+      <c r="AM67" s="5"/>
+      <c r="AN67" s="5"/>
+      <c r="AO67" s="5"/>
+      <c r="AP67" s="5"/>
+      <c r="AQ67" s="5"/>
+      <c r="AR67" s="5"/>
+      <c r="AS67" s="5"/>
+      <c r="AT67" s="5"/>
+      <c r="AU67" s="5"/>
+      <c r="AV67" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AW67" s="9"/>
+      <c r="AX67" s="9"/>
+      <c r="AY67" s="9"/>
+      <c r="AZ67" s="9"/>
+      <c r="BA67" s="9"/>
+      <c r="BB67" s="9"/>
+      <c r="BC67" s="9"/>
+      <c r="BD67" s="9"/>
+      <c r="BE67" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A68" s="11"/>
+      <c r="E68" t="s">
+        <v>82</v>
+      </c>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="5"/>
+      <c r="O68" s="5"/>
+      <c r="P68" s="5"/>
+      <c r="Q68" s="5"/>
+      <c r="R68" s="5"/>
+      <c r="S68" s="5"/>
+      <c r="T68" s="5"/>
+      <c r="U68" s="5"/>
+      <c r="V68" s="5"/>
+      <c r="W68" s="5"/>
+      <c r="X68" s="5"/>
+      <c r="Y68" s="5"/>
+      <c r="Z68" s="5"/>
+      <c r="AA68" s="5"/>
+      <c r="AB68" s="5"/>
+      <c r="AC68" s="5"/>
+      <c r="AD68" s="5"/>
+      <c r="AE68" s="5"/>
+      <c r="AF68" s="5"/>
+      <c r="AG68" s="5"/>
+      <c r="AH68" s="5"/>
+      <c r="AI68" s="5"/>
+      <c r="AJ68" s="5"/>
+      <c r="AK68" s="5"/>
+      <c r="AL68" s="5"/>
+      <c r="AM68" s="5"/>
+      <c r="AN68" s="5"/>
+      <c r="AO68" s="5"/>
+      <c r="AP68" s="5"/>
+      <c r="AQ68" s="5"/>
+      <c r="AR68" s="5"/>
+      <c r="AS68" s="5"/>
+      <c r="AT68" s="5"/>
+      <c r="AU68" s="5"/>
+      <c r="AV68" s="5"/>
+      <c r="AW68" s="5"/>
+      <c r="AX68" s="5"/>
+      <c r="AY68" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AZ68" s="9"/>
+      <c r="BA68" s="9"/>
+      <c r="BB68" s="9"/>
+      <c r="BC68" s="9"/>
+      <c r="BD68" s="9"/>
+      <c r="BE68" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="69" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>5</v>
       </c>
-      <c r="BE61" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="62" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="BE62" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="63" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="BE63" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="64" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="BE69" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BE70" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="71" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="BE71" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="72" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>12</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B72" t="s">
         <v>1</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E72" t="s">
         <v>13</v>
       </c>
-      <c r="F64" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE64" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="65" spans="5:57" x14ac:dyDescent="0.25">
-      <c r="E65" t="s">
+      <c r="F72" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE72" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="73" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
         <v>15</v>
       </c>
-      <c r="F65" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE65" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="66" spans="5:57" x14ac:dyDescent="0.25">
-      <c r="E66" t="s">
+      <c r="F73" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE73" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="74" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="E74" t="s">
         <v>16</v>
       </c>
-      <c r="F66" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE66" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="5:57" x14ac:dyDescent="0.25">
-      <c r="E67" t="s">
+      <c r="F74" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE74" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="75" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="E75" t="s">
         <v>17</v>
       </c>
-      <c r="F67" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE67" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="68" spans="5:57" x14ac:dyDescent="0.25">
-      <c r="E68" t="s">
+      <c r="F75" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE75" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="76" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="E76" t="s">
         <v>18</v>
       </c>
-      <c r="F68" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE68" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="69" spans="5:57" x14ac:dyDescent="0.25">
-      <c r="E69" t="s">
+      <c r="F76" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE76" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="77" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="E77" t="s">
         <v>31</v>
       </c>
-      <c r="P69" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE69" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="70" spans="5:57" x14ac:dyDescent="0.25">
-      <c r="E70" t="s">
+      <c r="P77" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE77" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="78" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
         <v>32</v>
       </c>
-      <c r="U70" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE70" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="71" spans="5:57" x14ac:dyDescent="0.25">
-      <c r="E71" t="s">
+      <c r="U78" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE78" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="79" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="E79" t="s">
         <v>33</v>
       </c>
-      <c r="U71" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE71" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="72" spans="5:57" x14ac:dyDescent="0.25">
-      <c r="E72" t="s">
+      <c r="U79" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE79" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="80" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="E80" t="s">
         <v>34</v>
       </c>
-      <c r="U72" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE72" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="73" spans="5:57" x14ac:dyDescent="0.25">
-      <c r="E73" t="s">
-        <v>35</v>
-      </c>
-      <c r="U73" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE73" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="74" spans="5:57" x14ac:dyDescent="0.25">
-      <c r="E74" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z74" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE74" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="75" spans="5:57" x14ac:dyDescent="0.25">
-      <c r="E75" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z75" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE75" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="76" spans="5:57" x14ac:dyDescent="0.25">
-      <c r="E76" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE76" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE76" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="77" spans="5:57" x14ac:dyDescent="0.25">
-      <c r="E77" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ77" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE77" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="78" spans="5:57" x14ac:dyDescent="0.25">
-      <c r="E78" t="s">
-        <v>40</v>
-      </c>
-      <c r="AO78" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE78" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="79" spans="5:57" x14ac:dyDescent="0.25">
-      <c r="E79" t="s">
-        <v>42</v>
-      </c>
-      <c r="AO79" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE79" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="80" spans="5:57" x14ac:dyDescent="0.25">
-      <c r="E80" t="s">
-        <v>41</v>
-      </c>
-      <c r="AT80" t="s">
+      <c r="U80" t="s">
         <v>14</v>
       </c>
       <c r="BE80" t="s">
@@ -3751,9 +4146,9 @@
     </row>
     <row r="81" spans="1:57" x14ac:dyDescent="0.25">
       <c r="E81" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT81" t="s">
+        <v>35</v>
+      </c>
+      <c r="U81" t="s">
         <v>14</v>
       </c>
       <c r="BE81" t="s">
@@ -3762,34 +4157,122 @@
     </row>
     <row r="82" spans="1:57" x14ac:dyDescent="0.25">
       <c r="E82" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z82" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE82" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="83" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="E83" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z83" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE83" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="84" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="E84" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE84" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE84" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="85" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="E85" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ85" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE85" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="86" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="E86" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO86" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE86" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="87" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="E87" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO87" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE87" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="88" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="E88" t="s">
+        <v>41</v>
+      </c>
+      <c r="AT88" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE88" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="89" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="E89" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT89" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE89" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="90" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="E90" t="s">
         <v>44</v>
       </c>
-      <c r="BD82" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE82" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="83" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
+      <c r="BD90" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE90" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="91" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
         <v>21</v>
       </c>
-      <c r="L83" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE83" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="84" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="L91" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE91" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="92" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>19</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E92" t="s">
         <v>20</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F92" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest save of release docs
</commit_message>
<xml_diff>
--- a/ReleaseTimelines.xlsx
+++ b/ReleaseTimelines.xlsx
@@ -709,10 +709,10 @@
   <dimension ref="A1:BE92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F50" sqref="F50"/>
+      <selection pane="bottomRight" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Hosting dates and speeds documented
</commit_message>
<xml_diff>
--- a/ReleaseTimelines.xlsx
+++ b/ReleaseTimelines.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="97">
   <si>
     <t>Dev</t>
   </si>
@@ -251,6 +251,9 @@
     <t>Remote Support</t>
   </si>
   <si>
+    <t>Specialist</t>
+  </si>
+  <si>
     <t>Dial-up 56 Kbps</t>
   </si>
   <si>
@@ -309,6 +312,9 @@
   </si>
   <si>
     <t>T4 274 Mbps</t>
+  </si>
+  <si>
+    <t>ARKANET</t>
   </si>
 </sst>
 </file>
@@ -324,7 +330,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,6 +397,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -404,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -426,6 +438,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,13 +719,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE92"/>
+  <dimension ref="A1:BE93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B50" sqref="B50"/>
+      <selection pane="bottomRight" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2874,30 +2887,28 @@
         <v>34</v>
       </c>
       <c r="C50" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="E50" t="s">
-        <v>83</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="5"/>
-      <c r="L50" s="5"/>
-      <c r="M50" s="5"/>
-      <c r="N50" s="5"/>
-      <c r="O50" s="5"/>
-      <c r="P50" s="5"/>
-      <c r="Q50" s="5"/>
-      <c r="R50" s="5"/>
-      <c r="S50" s="5"/>
-      <c r="T50" s="12" t="s">
-        <v>14</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+      <c r="K50" s="12"/>
+      <c r="L50" s="12"/>
+      <c r="M50" s="12"/>
+      <c r="N50" s="12"/>
+      <c r="O50" s="12"/>
+      <c r="P50" s="12"/>
+      <c r="Q50" s="12"/>
+      <c r="R50" s="12"/>
+      <c r="S50" s="12"/>
+      <c r="T50" s="12"/>
       <c r="U50" s="12"/>
       <c r="V50" s="12"/>
       <c r="W50" s="12"/>
@@ -2941,7 +2952,7 @@
     <row r="51" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="E51" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
@@ -2949,21 +2960,21 @@
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
-      <c r="O51" s="5"/>
-      <c r="P51" s="5"/>
-      <c r="Q51" s="5"/>
-      <c r="R51" s="5"/>
-      <c r="S51" s="5"/>
-      <c r="T51" s="5"/>
-      <c r="U51" s="5"/>
-      <c r="V51" s="5"/>
-      <c r="W51" s="5"/>
-      <c r="X51" s="12" t="s">
-        <v>14</v>
-      </c>
+      <c r="L51" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="M51" s="12"/>
+      <c r="N51" s="12"/>
+      <c r="O51" s="12"/>
+      <c r="P51" s="12"/>
+      <c r="Q51" s="12"/>
+      <c r="R51" s="12"/>
+      <c r="S51" s="12"/>
+      <c r="T51" s="12"/>
+      <c r="U51" s="12"/>
+      <c r="V51" s="12"/>
+      <c r="W51" s="12"/>
+      <c r="X51" s="12"/>
       <c r="Y51" s="12"/>
       <c r="Z51" s="12"/>
       <c r="AA51" s="12"/>
@@ -3003,7 +3014,7 @@
     <row r="52" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="E52" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
@@ -3014,15 +3025,17 @@
       <c r="L52" s="5"/>
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
-      <c r="O52" s="5"/>
-      <c r="P52" s="5"/>
-      <c r="Q52" s="5"/>
-      <c r="R52" s="5"/>
-      <c r="S52" s="5"/>
-      <c r="T52" s="5"/>
-      <c r="U52" s="5"/>
-      <c r="V52" s="5"/>
-      <c r="W52" s="5"/>
+      <c r="O52" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="P52" s="12"/>
+      <c r="Q52" s="12"/>
+      <c r="R52" s="12"/>
+      <c r="S52" s="12"/>
+      <c r="T52" s="12"/>
+      <c r="U52" s="12"/>
+      <c r="V52" s="12"/>
+      <c r="W52" s="12"/>
       <c r="X52" s="12"/>
       <c r="Y52" s="12"/>
       <c r="Z52" s="12"/>
@@ -3056,12 +3069,14 @@
       <c r="BB52" s="12"/>
       <c r="BC52" s="12"/>
       <c r="BD52" s="12"/>
-      <c r="BE52" s="12"/>
+      <c r="BE52" s="12" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="53" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A53" s="11"/>
       <c r="E53" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
@@ -3081,10 +3096,12 @@
       <c r="U53" s="5"/>
       <c r="V53" s="5"/>
       <c r="W53" s="5"/>
-      <c r="X53" s="12"/>
-      <c r="Y53" s="12"/>
-      <c r="Z53" s="12"/>
-      <c r="AA53" s="12"/>
+      <c r="X53" s="5"/>
+      <c r="Y53" s="5"/>
+      <c r="Z53" s="5"/>
+      <c r="AA53" s="12" t="s">
+        <v>14</v>
+      </c>
       <c r="AB53" s="12"/>
       <c r="AC53" s="12"/>
       <c r="AD53" s="12"/>
@@ -3114,74 +3131,79 @@
       <c r="BB53" s="12"/>
       <c r="BC53" s="12"/>
       <c r="BD53" s="12"/>
-      <c r="BE53" s="12"/>
+      <c r="BE53" s="12" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="54" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
+      <c r="C54" t="s">
+        <v>4</v>
+      </c>
       <c r="E54" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-      <c r="J54" s="5"/>
-      <c r="K54" s="5"/>
-      <c r="L54" s="5"/>
-      <c r="M54" s="5"/>
-      <c r="N54" s="5"/>
-      <c r="O54" s="5"/>
-      <c r="P54" s="5"/>
-      <c r="Q54" s="5"/>
-      <c r="R54" s="5"/>
-      <c r="S54" s="5"/>
-      <c r="T54" s="5"/>
-      <c r="U54" s="5"/>
-      <c r="V54" s="5"/>
-      <c r="W54" s="5"/>
-      <c r="X54" s="5"/>
-      <c r="Y54" s="5"/>
-      <c r="Z54" s="5"/>
-      <c r="AA54" s="5"/>
-      <c r="AB54" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC54" s="12"/>
-      <c r="AD54" s="12"/>
-      <c r="AE54" s="12"/>
-      <c r="AF54" s="12"/>
-      <c r="AG54" s="12"/>
-      <c r="AH54" s="12"/>
-      <c r="AI54" s="12"/>
-      <c r="AJ54" s="12"/>
-      <c r="AK54" s="12"/>
-      <c r="AL54" s="12"/>
-      <c r="AM54" s="12"/>
-      <c r="AN54" s="12"/>
-      <c r="AO54" s="12"/>
-      <c r="AP54" s="12"/>
-      <c r="AQ54" s="12"/>
-      <c r="AR54" s="12"/>
-      <c r="AS54" s="12"/>
-      <c r="AT54" s="12"/>
-      <c r="AU54" s="12"/>
-      <c r="AV54" s="12"/>
-      <c r="AW54" s="12"/>
-      <c r="AX54" s="12"/>
-      <c r="AY54" s="12"/>
-      <c r="AZ54" s="12"/>
-      <c r="BA54" s="12"/>
-      <c r="BB54" s="12"/>
-      <c r="BC54" s="12"/>
-      <c r="BD54" s="12"/>
-      <c r="BE54" s="12" t="s">
+      <c r="I54" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J54" s="9"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
+      <c r="N54" s="9"/>
+      <c r="O54" s="9"/>
+      <c r="P54" s="9"/>
+      <c r="Q54" s="9"/>
+      <c r="R54" s="9"/>
+      <c r="S54" s="9"/>
+      <c r="T54" s="9"/>
+      <c r="U54" s="9"/>
+      <c r="V54" s="9"/>
+      <c r="W54" s="9"/>
+      <c r="X54" s="9"/>
+      <c r="Y54" s="9"/>
+      <c r="Z54" s="9"/>
+      <c r="AA54" s="9"/>
+      <c r="AB54" s="9"/>
+      <c r="AC54" s="9"/>
+      <c r="AD54" s="9"/>
+      <c r="AE54" s="9"/>
+      <c r="AF54" s="9"/>
+      <c r="AG54" s="9"/>
+      <c r="AH54" s="9"/>
+      <c r="AI54" s="9"/>
+      <c r="AJ54" s="9"/>
+      <c r="AK54" s="9"/>
+      <c r="AL54" s="9"/>
+      <c r="AM54" s="9"/>
+      <c r="AN54" s="9"/>
+      <c r="AO54" s="9"/>
+      <c r="AP54" s="9"/>
+      <c r="AQ54" s="9"/>
+      <c r="AR54" s="9"/>
+      <c r="AS54" s="9"/>
+      <c r="AT54" s="9"/>
+      <c r="AU54" s="9"/>
+      <c r="AV54" s="9"/>
+      <c r="AW54" s="9"/>
+      <c r="AX54" s="9"/>
+      <c r="AY54" s="9"/>
+      <c r="AZ54" s="9"/>
+      <c r="BA54" s="9"/>
+      <c r="BB54" s="9"/>
+      <c r="BC54" s="9"/>
+      <c r="BD54" s="9"/>
+      <c r="BE54" s="9" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A55" s="11"/>
       <c r="E55" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
@@ -3195,51 +3217,55 @@
       <c r="O55" s="5"/>
       <c r="P55" s="5"/>
       <c r="Q55" s="5"/>
-      <c r="R55" s="5"/>
-      <c r="S55" s="5"/>
-      <c r="T55" s="5"/>
-      <c r="U55" s="5"/>
-      <c r="V55" s="5"/>
-      <c r="W55" s="5"/>
-      <c r="X55" s="5"/>
-      <c r="Y55" s="5"/>
-      <c r="Z55" s="5"/>
-      <c r="AA55" s="5"/>
-      <c r="AB55" s="12"/>
-      <c r="AC55" s="12"/>
-      <c r="AD55" s="12"/>
-      <c r="AE55" s="12"/>
-      <c r="AF55" s="12"/>
-      <c r="AG55" s="12"/>
-      <c r="AH55" s="12"/>
-      <c r="AI55" s="12"/>
-      <c r="AJ55" s="12"/>
-      <c r="AK55" s="12"/>
-      <c r="AL55" s="12"/>
-      <c r="AM55" s="12"/>
-      <c r="AN55" s="12"/>
-      <c r="AO55" s="12"/>
-      <c r="AP55" s="12"/>
-      <c r="AQ55" s="12"/>
-      <c r="AR55" s="12"/>
-      <c r="AS55" s="12"/>
-      <c r="AT55" s="12"/>
-      <c r="AU55" s="12"/>
-      <c r="AV55" s="12"/>
-      <c r="AW55" s="12"/>
-      <c r="AX55" s="12"/>
-      <c r="AY55" s="12"/>
-      <c r="AZ55" s="12"/>
-      <c r="BA55" s="12"/>
-      <c r="BB55" s="12"/>
-      <c r="BC55" s="12"/>
-      <c r="BD55" s="12"/>
-      <c r="BE55" s="12"/>
+      <c r="R55" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="S55" s="9"/>
+      <c r="T55" s="9"/>
+      <c r="U55" s="9"/>
+      <c r="V55" s="9"/>
+      <c r="W55" s="9"/>
+      <c r="X55" s="9"/>
+      <c r="Y55" s="9"/>
+      <c r="Z55" s="9"/>
+      <c r="AA55" s="9"/>
+      <c r="AB55" s="9"/>
+      <c r="AC55" s="9"/>
+      <c r="AD55" s="9"/>
+      <c r="AE55" s="9"/>
+      <c r="AF55" s="9"/>
+      <c r="AG55" s="9"/>
+      <c r="AH55" s="9"/>
+      <c r="AI55" s="9"/>
+      <c r="AJ55" s="9"/>
+      <c r="AK55" s="9"/>
+      <c r="AL55" s="9"/>
+      <c r="AM55" s="9"/>
+      <c r="AN55" s="9"/>
+      <c r="AO55" s="9"/>
+      <c r="AP55" s="9"/>
+      <c r="AQ55" s="9"/>
+      <c r="AR55" s="9"/>
+      <c r="AS55" s="9"/>
+      <c r="AT55" s="9"/>
+      <c r="AU55" s="9"/>
+      <c r="AV55" s="9"/>
+      <c r="AW55" s="9"/>
+      <c r="AX55" s="9"/>
+      <c r="AY55" s="9"/>
+      <c r="AZ55" s="9"/>
+      <c r="BA55" s="9"/>
+      <c r="BB55" s="9"/>
+      <c r="BC55" s="9"/>
+      <c r="BD55" s="9"/>
+      <c r="BE55" s="9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="56" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A56" s="11"/>
       <c r="E56" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
@@ -3256,43 +3282,47 @@
       <c r="R56" s="5"/>
       <c r="S56" s="5"/>
       <c r="T56" s="5"/>
-      <c r="U56" s="5"/>
-      <c r="V56" s="5"/>
-      <c r="W56" s="5"/>
-      <c r="X56" s="5"/>
-      <c r="Y56" s="5"/>
-      <c r="Z56" s="5"/>
-      <c r="AA56" s="5"/>
-      <c r="AB56" s="12"/>
-      <c r="AC56" s="12"/>
-      <c r="AD56" s="12"/>
-      <c r="AE56" s="12"/>
-      <c r="AF56" s="12"/>
-      <c r="AG56" s="12"/>
-      <c r="AH56" s="12"/>
-      <c r="AI56" s="12"/>
-      <c r="AJ56" s="12"/>
-      <c r="AK56" s="12"/>
-      <c r="AL56" s="12"/>
-      <c r="AM56" s="12"/>
-      <c r="AN56" s="12"/>
-      <c r="AO56" s="12"/>
-      <c r="AP56" s="12"/>
-      <c r="AQ56" s="12"/>
-      <c r="AR56" s="12"/>
-      <c r="AS56" s="12"/>
-      <c r="AT56" s="12"/>
-      <c r="AU56" s="12"/>
-      <c r="AV56" s="12"/>
-      <c r="AW56" s="12"/>
-      <c r="AX56" s="12"/>
-      <c r="AY56" s="12"/>
-      <c r="AZ56" s="12"/>
-      <c r="BA56" s="12"/>
-      <c r="BB56" s="12"/>
-      <c r="BC56" s="12"/>
-      <c r="BD56" s="12"/>
-      <c r="BE56" s="12"/>
+      <c r="U56" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="V56" s="9"/>
+      <c r="W56" s="9"/>
+      <c r="X56" s="9"/>
+      <c r="Y56" s="9"/>
+      <c r="Z56" s="9"/>
+      <c r="AA56" s="9"/>
+      <c r="AB56" s="9"/>
+      <c r="AC56" s="9"/>
+      <c r="AD56" s="9"/>
+      <c r="AE56" s="9"/>
+      <c r="AF56" s="9"/>
+      <c r="AG56" s="9"/>
+      <c r="AH56" s="9"/>
+      <c r="AI56" s="9"/>
+      <c r="AJ56" s="9"/>
+      <c r="AK56" s="9"/>
+      <c r="AL56" s="9"/>
+      <c r="AM56" s="9"/>
+      <c r="AN56" s="9"/>
+      <c r="AO56" s="9"/>
+      <c r="AP56" s="9"/>
+      <c r="AQ56" s="9"/>
+      <c r="AR56" s="9"/>
+      <c r="AS56" s="9"/>
+      <c r="AT56" s="9"/>
+      <c r="AU56" s="9"/>
+      <c r="AV56" s="9"/>
+      <c r="AW56" s="9"/>
+      <c r="AX56" s="9"/>
+      <c r="AY56" s="9"/>
+      <c r="AZ56" s="9"/>
+      <c r="BA56" s="9"/>
+      <c r="BB56" s="9"/>
+      <c r="BC56" s="9"/>
+      <c r="BD56" s="9"/>
+      <c r="BE56" s="9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="57" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A57" s="11"/>
@@ -3317,45 +3347,49 @@
       <c r="U57" s="5"/>
       <c r="V57" s="5"/>
       <c r="W57" s="5"/>
-      <c r="X57" s="5"/>
-      <c r="Y57" s="5"/>
-      <c r="Z57" s="5"/>
-      <c r="AA57" s="5"/>
-      <c r="AB57" s="12"/>
-      <c r="AC57" s="12"/>
-      <c r="AD57" s="12"/>
-      <c r="AE57" s="12"/>
-      <c r="AF57" s="12"/>
-      <c r="AG57" s="12"/>
-      <c r="AH57" s="12"/>
-      <c r="AI57" s="12"/>
-      <c r="AJ57" s="12"/>
-      <c r="AK57" s="12"/>
-      <c r="AL57" s="12"/>
-      <c r="AM57" s="12"/>
-      <c r="AN57" s="12"/>
-      <c r="AO57" s="12"/>
-      <c r="AP57" s="12"/>
-      <c r="AQ57" s="12"/>
-      <c r="AR57" s="12"/>
-      <c r="AS57" s="12"/>
-      <c r="AT57" s="12"/>
-      <c r="AU57" s="12"/>
-      <c r="AV57" s="12"/>
-      <c r="AW57" s="12"/>
-      <c r="AX57" s="12"/>
-      <c r="AY57" s="12"/>
-      <c r="AZ57" s="12"/>
-      <c r="BA57" s="12"/>
-      <c r="BB57" s="12"/>
-      <c r="BC57" s="12"/>
-      <c r="BD57" s="12"/>
-      <c r="BE57" s="12"/>
+      <c r="X57" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y57" s="9"/>
+      <c r="Z57" s="9"/>
+      <c r="AA57" s="9"/>
+      <c r="AB57" s="9"/>
+      <c r="AC57" s="9"/>
+      <c r="AD57" s="9"/>
+      <c r="AE57" s="9"/>
+      <c r="AF57" s="9"/>
+      <c r="AG57" s="9"/>
+      <c r="AH57" s="9"/>
+      <c r="AI57" s="9"/>
+      <c r="AJ57" s="9"/>
+      <c r="AK57" s="9"/>
+      <c r="AL57" s="9"/>
+      <c r="AM57" s="9"/>
+      <c r="AN57" s="9"/>
+      <c r="AO57" s="9"/>
+      <c r="AP57" s="9"/>
+      <c r="AQ57" s="9"/>
+      <c r="AR57" s="9"/>
+      <c r="AS57" s="9"/>
+      <c r="AT57" s="9"/>
+      <c r="AU57" s="9"/>
+      <c r="AV57" s="9"/>
+      <c r="AW57" s="9"/>
+      <c r="AX57" s="9"/>
+      <c r="AY57" s="9"/>
+      <c r="AZ57" s="9"/>
+      <c r="BA57" s="9"/>
+      <c r="BB57" s="9"/>
+      <c r="BC57" s="9"/>
+      <c r="BD57" s="9"/>
+      <c r="BE57" s="9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="58" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
       <c r="E58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
@@ -3379,36 +3413,40 @@
       <c r="Y58" s="5"/>
       <c r="Z58" s="5"/>
       <c r="AA58" s="5"/>
-      <c r="AB58" s="12"/>
-      <c r="AC58" s="12"/>
-      <c r="AD58" s="12"/>
-      <c r="AE58" s="12"/>
-      <c r="AF58" s="12"/>
-      <c r="AG58" s="12"/>
-      <c r="AH58" s="12"/>
-      <c r="AI58" s="12"/>
-      <c r="AJ58" s="12"/>
-      <c r="AK58" s="12"/>
-      <c r="AL58" s="12"/>
-      <c r="AM58" s="12"/>
-      <c r="AN58" s="12"/>
-      <c r="AO58" s="12"/>
-      <c r="AP58" s="12"/>
-      <c r="AQ58" s="12"/>
-      <c r="AR58" s="12"/>
-      <c r="AS58" s="12"/>
-      <c r="AT58" s="12"/>
-      <c r="AU58" s="12"/>
-      <c r="AV58" s="12"/>
-      <c r="AW58" s="12"/>
-      <c r="AX58" s="12"/>
-      <c r="AY58" s="12"/>
-      <c r="AZ58" s="12"/>
-      <c r="BA58" s="12"/>
-      <c r="BB58" s="12"/>
-      <c r="BC58" s="12"/>
-      <c r="BD58" s="12"/>
-      <c r="BE58" s="12"/>
+      <c r="AB58" s="5"/>
+      <c r="AC58" s="5"/>
+      <c r="AD58" s="5"/>
+      <c r="AE58" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF58" s="9"/>
+      <c r="AG58" s="9"/>
+      <c r="AH58" s="9"/>
+      <c r="AI58" s="9"/>
+      <c r="AJ58" s="9"/>
+      <c r="AK58" s="9"/>
+      <c r="AL58" s="9"/>
+      <c r="AM58" s="9"/>
+      <c r="AN58" s="9"/>
+      <c r="AO58" s="9"/>
+      <c r="AP58" s="9"/>
+      <c r="AQ58" s="9"/>
+      <c r="AR58" s="9"/>
+      <c r="AS58" s="9"/>
+      <c r="AT58" s="9"/>
+      <c r="AU58" s="9"/>
+      <c r="AV58" s="9"/>
+      <c r="AW58" s="9"/>
+      <c r="AX58" s="9"/>
+      <c r="AY58" s="9"/>
+      <c r="AZ58" s="9"/>
+      <c r="BA58" s="9"/>
+      <c r="BB58" s="9"/>
+      <c r="BC58" s="9"/>
+      <c r="BD58" s="9"/>
+      <c r="BE58" s="9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="59" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
@@ -3437,36 +3475,40 @@
       <c r="Y59" s="5"/>
       <c r="Z59" s="5"/>
       <c r="AA59" s="5"/>
-      <c r="AB59" s="12"/>
-      <c r="AC59" s="12"/>
-      <c r="AD59" s="12"/>
-      <c r="AE59" s="12"/>
-      <c r="AF59" s="12"/>
-      <c r="AG59" s="12"/>
-      <c r="AH59" s="12"/>
-      <c r="AI59" s="12"/>
-      <c r="AJ59" s="12"/>
-      <c r="AK59" s="12"/>
-      <c r="AL59" s="12"/>
-      <c r="AM59" s="12"/>
-      <c r="AN59" s="12"/>
-      <c r="AO59" s="12"/>
-      <c r="AP59" s="12"/>
-      <c r="AQ59" s="12"/>
-      <c r="AR59" s="12"/>
-      <c r="AS59" s="12"/>
-      <c r="AT59" s="12"/>
-      <c r="AU59" s="12"/>
-      <c r="AV59" s="12"/>
-      <c r="AW59" s="12"/>
-      <c r="AX59" s="12"/>
-      <c r="AY59" s="12"/>
-      <c r="AZ59" s="12"/>
-      <c r="BA59" s="12"/>
-      <c r="BB59" s="12"/>
-      <c r="BC59" s="12"/>
-      <c r="BD59" s="12"/>
-      <c r="BE59" s="12"/>
+      <c r="AB59" s="5"/>
+      <c r="AC59" s="5"/>
+      <c r="AD59" s="5"/>
+      <c r="AE59" s="5"/>
+      <c r="AF59" s="5"/>
+      <c r="AG59" s="5"/>
+      <c r="AH59" s="5"/>
+      <c r="AI59" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ59" s="9"/>
+      <c r="AK59" s="9"/>
+      <c r="AL59" s="9"/>
+      <c r="AM59" s="9"/>
+      <c r="AN59" s="9"/>
+      <c r="AO59" s="9"/>
+      <c r="AP59" s="9"/>
+      <c r="AQ59" s="9"/>
+      <c r="AR59" s="9"/>
+      <c r="AS59" s="9"/>
+      <c r="AT59" s="9"/>
+      <c r="AU59" s="9"/>
+      <c r="AV59" s="9"/>
+      <c r="AW59" s="9"/>
+      <c r="AX59" s="9"/>
+      <c r="AY59" s="9"/>
+      <c r="AZ59" s="9"/>
+      <c r="BA59" s="9"/>
+      <c r="BB59" s="9"/>
+      <c r="BC59" s="9"/>
+      <c r="BD59" s="9"/>
+      <c r="BE59" s="9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="60" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A60" s="11"/>
@@ -3495,36 +3537,40 @@
       <c r="Y60" s="5"/>
       <c r="Z60" s="5"/>
       <c r="AA60" s="5"/>
-      <c r="AB60" s="12"/>
-      <c r="AC60" s="12"/>
-      <c r="AD60" s="12"/>
-      <c r="AE60" s="12"/>
-      <c r="AF60" s="12"/>
-      <c r="AG60" s="12"/>
-      <c r="AH60" s="12"/>
-      <c r="AI60" s="12"/>
-      <c r="AJ60" s="12"/>
-      <c r="AK60" s="12"/>
-      <c r="AL60" s="12"/>
-      <c r="AM60" s="12"/>
-      <c r="AN60" s="12"/>
-      <c r="AO60" s="12"/>
-      <c r="AP60" s="12"/>
-      <c r="AQ60" s="12"/>
-      <c r="AR60" s="12"/>
-      <c r="AS60" s="12"/>
-      <c r="AT60" s="12"/>
-      <c r="AU60" s="12"/>
-      <c r="AV60" s="12"/>
-      <c r="AW60" s="12"/>
-      <c r="AX60" s="12"/>
-      <c r="AY60" s="12"/>
-      <c r="AZ60" s="12"/>
-      <c r="BA60" s="12"/>
-      <c r="BB60" s="12"/>
-      <c r="BC60" s="12"/>
-      <c r="BD60" s="12"/>
-      <c r="BE60" s="12"/>
+      <c r="AB60" s="5"/>
+      <c r="AC60" s="5"/>
+      <c r="AD60" s="5"/>
+      <c r="AE60" s="5"/>
+      <c r="AF60" s="5"/>
+      <c r="AG60" s="5"/>
+      <c r="AH60" s="5"/>
+      <c r="AI60" s="5"/>
+      <c r="AJ60" s="5"/>
+      <c r="AK60" s="5"/>
+      <c r="AL60" s="5"/>
+      <c r="AM60" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN60" s="9"/>
+      <c r="AO60" s="9"/>
+      <c r="AP60" s="9"/>
+      <c r="AQ60" s="9"/>
+      <c r="AR60" s="9"/>
+      <c r="AS60" s="9"/>
+      <c r="AT60" s="9"/>
+      <c r="AU60" s="9"/>
+      <c r="AV60" s="9"/>
+      <c r="AW60" s="9"/>
+      <c r="AX60" s="9"/>
+      <c r="AY60" s="9"/>
+      <c r="AZ60" s="9"/>
+      <c r="BA60" s="9"/>
+      <c r="BB60" s="9"/>
+      <c r="BC60" s="9"/>
+      <c r="BD60" s="9"/>
+      <c r="BE60" s="9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="61" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A61" s="11"/>
@@ -3553,44 +3599,45 @@
       <c r="Y61" s="5"/>
       <c r="Z61" s="5"/>
       <c r="AA61" s="5"/>
-      <c r="AB61" s="12"/>
-      <c r="AC61" s="12"/>
-      <c r="AD61" s="12"/>
-      <c r="AE61" s="12"/>
-      <c r="AF61" s="12"/>
-      <c r="AG61" s="12"/>
-      <c r="AH61" s="12"/>
-      <c r="AI61" s="12"/>
-      <c r="AJ61" s="12"/>
-      <c r="AK61" s="12"/>
-      <c r="AL61" s="12"/>
-      <c r="AM61" s="12"/>
-      <c r="AN61" s="12"/>
-      <c r="AO61" s="12"/>
-      <c r="AP61" s="12"/>
-      <c r="AQ61" s="12"/>
-      <c r="AR61" s="12"/>
-      <c r="AS61" s="12"/>
-      <c r="AT61" s="12"/>
-      <c r="AU61" s="12"/>
-      <c r="AV61" s="12"/>
-      <c r="AW61" s="12"/>
-      <c r="AX61" s="12"/>
-      <c r="AY61" s="12"/>
-      <c r="AZ61" s="12"/>
-      <c r="BA61" s="12"/>
-      <c r="BB61" s="12"/>
-      <c r="BC61" s="12"/>
-      <c r="BD61" s="12"/>
-      <c r="BE61" s="12"/>
+      <c r="AB61" s="5"/>
+      <c r="AC61" s="5"/>
+      <c r="AD61" s="5"/>
+      <c r="AE61" s="5"/>
+      <c r="AF61" s="5"/>
+      <c r="AG61" s="5"/>
+      <c r="AH61" s="5"/>
+      <c r="AI61" s="5"/>
+      <c r="AJ61" s="5"/>
+      <c r="AK61" s="5"/>
+      <c r="AL61" s="5"/>
+      <c r="AM61" s="5"/>
+      <c r="AN61" s="5"/>
+      <c r="AO61" s="5"/>
+      <c r="AP61" s="5"/>
+      <c r="AQ61" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AR61" s="9"/>
+      <c r="AS61" s="9"/>
+      <c r="AT61" s="9"/>
+      <c r="AU61" s="9"/>
+      <c r="AV61" s="9"/>
+      <c r="AW61" s="9"/>
+      <c r="AX61" s="9"/>
+      <c r="AY61" s="9"/>
+      <c r="AZ61" s="9"/>
+      <c r="BA61" s="9"/>
+      <c r="BB61" s="9"/>
+      <c r="BC61" s="9"/>
+      <c r="BD61" s="9"/>
+      <c r="BE61" s="9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="62" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
-      <c r="C62" t="s">
-        <v>76</v>
-      </c>
       <c r="E62" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
@@ -3614,28 +3661,28 @@
       <c r="Y62" s="5"/>
       <c r="Z62" s="5"/>
       <c r="AA62" s="5"/>
-      <c r="AB62" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC62" s="9"/>
-      <c r="AD62" s="9"/>
-      <c r="AE62" s="9"/>
-      <c r="AF62" s="9"/>
-      <c r="AG62" s="9"/>
-      <c r="AH62" s="9"/>
-      <c r="AI62" s="9"/>
-      <c r="AJ62" s="9"/>
-      <c r="AK62" s="9"/>
-      <c r="AL62" s="9"/>
-      <c r="AM62" s="9"/>
-      <c r="AN62" s="9"/>
-      <c r="AO62" s="9"/>
-      <c r="AP62" s="9"/>
-      <c r="AQ62" s="9"/>
-      <c r="AR62" s="9"/>
-      <c r="AS62" s="9"/>
-      <c r="AT62" s="9"/>
-      <c r="AU62" s="9"/>
+      <c r="AB62" s="5"/>
+      <c r="AC62" s="5"/>
+      <c r="AD62" s="5"/>
+      <c r="AE62" s="5"/>
+      <c r="AF62" s="5"/>
+      <c r="AG62" s="5"/>
+      <c r="AH62" s="5"/>
+      <c r="AI62" s="5"/>
+      <c r="AJ62" s="5"/>
+      <c r="AK62" s="5"/>
+      <c r="AL62" s="5"/>
+      <c r="AM62" s="5"/>
+      <c r="AN62" s="5"/>
+      <c r="AO62" s="5"/>
+      <c r="AP62" s="5"/>
+      <c r="AQ62" s="5"/>
+      <c r="AR62" s="5"/>
+      <c r="AS62" s="5"/>
+      <c r="AT62" s="5"/>
+      <c r="AU62" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="AV62" s="9"/>
       <c r="AW62" s="9"/>
       <c r="AX62" s="9"/>
@@ -3651,8 +3698,11 @@
     </row>
     <row r="63" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
+      <c r="C63" t="s">
+        <v>77</v>
+      </c>
       <c r="E63" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
@@ -3677,44 +3727,44 @@
       <c r="Z63" s="5"/>
       <c r="AA63" s="5"/>
       <c r="AB63" s="5"/>
-      <c r="AC63" s="5"/>
-      <c r="AD63" s="5"/>
-      <c r="AE63" s="5"/>
-      <c r="AF63" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG63" s="9"/>
-      <c r="AH63" s="9"/>
-      <c r="AI63" s="9"/>
-      <c r="AJ63" s="9"/>
-      <c r="AK63" s="9"/>
-      <c r="AL63" s="9"/>
-      <c r="AM63" s="9"/>
-      <c r="AN63" s="9"/>
-      <c r="AO63" s="9"/>
-      <c r="AP63" s="9"/>
-      <c r="AQ63" s="9"/>
-      <c r="AR63" s="9"/>
-      <c r="AS63" s="9"/>
-      <c r="AT63" s="9"/>
-      <c r="AU63" s="9"/>
-      <c r="AV63" s="9"/>
-      <c r="AW63" s="9"/>
-      <c r="AX63" s="9"/>
-      <c r="AY63" s="9"/>
-      <c r="AZ63" s="9"/>
-      <c r="BA63" s="9"/>
-      <c r="BB63" s="9"/>
-      <c r="BC63" s="9"/>
-      <c r="BD63" s="9"/>
-      <c r="BE63" s="9" t="s">
+      <c r="AC63" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD63" s="13"/>
+      <c r="AE63" s="13"/>
+      <c r="AF63" s="13"/>
+      <c r="AG63" s="13"/>
+      <c r="AH63" s="13"/>
+      <c r="AI63" s="13"/>
+      <c r="AJ63" s="13"/>
+      <c r="AK63" s="13"/>
+      <c r="AL63" s="13"/>
+      <c r="AM63" s="13"/>
+      <c r="AN63" s="13"/>
+      <c r="AO63" s="13"/>
+      <c r="AP63" s="13"/>
+      <c r="AQ63" s="13"/>
+      <c r="AR63" s="13"/>
+      <c r="AS63" s="13"/>
+      <c r="AT63" s="13"/>
+      <c r="AU63" s="13"/>
+      <c r="AV63" s="13"/>
+      <c r="AW63" s="13"/>
+      <c r="AX63" s="13"/>
+      <c r="AY63" s="13"/>
+      <c r="AZ63" s="13"/>
+      <c r="BA63" s="13"/>
+      <c r="BB63" s="13"/>
+      <c r="BC63" s="13"/>
+      <c r="BD63" s="13"/>
+      <c r="BE63" s="13" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A64" s="11"/>
       <c r="E64" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
@@ -3743,40 +3793,40 @@
       <c r="AD64" s="5"/>
       <c r="AE64" s="5"/>
       <c r="AF64" s="5"/>
-      <c r="AG64" s="5"/>
-      <c r="AH64" s="5"/>
-      <c r="AI64" s="5"/>
-      <c r="AJ64" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AK64" s="9"/>
-      <c r="AL64" s="9"/>
-      <c r="AM64" s="9"/>
-      <c r="AN64" s="9"/>
-      <c r="AO64" s="9"/>
-      <c r="AP64" s="9"/>
-      <c r="AQ64" s="9"/>
-      <c r="AR64" s="9"/>
-      <c r="AS64" s="9"/>
-      <c r="AT64" s="9"/>
-      <c r="AU64" s="9"/>
-      <c r="AV64" s="9"/>
-      <c r="AW64" s="9"/>
-      <c r="AX64" s="9"/>
-      <c r="AY64" s="9"/>
-      <c r="AZ64" s="9"/>
-      <c r="BA64" s="9"/>
-      <c r="BB64" s="9"/>
-      <c r="BC64" s="9"/>
-      <c r="BD64" s="9"/>
-      <c r="BE64" s="9" t="s">
+      <c r="AG64" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH64" s="13"/>
+      <c r="AI64" s="13"/>
+      <c r="AJ64" s="13"/>
+      <c r="AK64" s="13"/>
+      <c r="AL64" s="13"/>
+      <c r="AM64" s="13"/>
+      <c r="AN64" s="13"/>
+      <c r="AO64" s="13"/>
+      <c r="AP64" s="13"/>
+      <c r="AQ64" s="13"/>
+      <c r="AR64" s="13"/>
+      <c r="AS64" s="13"/>
+      <c r="AT64" s="13"/>
+      <c r="AU64" s="13"/>
+      <c r="AV64" s="13"/>
+      <c r="AW64" s="13"/>
+      <c r="AX64" s="13"/>
+      <c r="AY64" s="13"/>
+      <c r="AZ64" s="13"/>
+      <c r="BA64" s="13"/>
+      <c r="BB64" s="13"/>
+      <c r="BC64" s="13"/>
+      <c r="BD64" s="13"/>
+      <c r="BE64" s="13" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="65" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A65" s="11"/>
       <c r="E65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
@@ -3809,36 +3859,36 @@
       <c r="AH65" s="5"/>
       <c r="AI65" s="5"/>
       <c r="AJ65" s="5"/>
-      <c r="AK65" s="5"/>
-      <c r="AL65" s="5"/>
-      <c r="AM65" s="5"/>
-      <c r="AN65" s="5"/>
-      <c r="AO65" s="5"/>
-      <c r="AP65" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AQ65" s="9"/>
-      <c r="AR65" s="9"/>
-      <c r="AS65" s="9"/>
-      <c r="AT65" s="9"/>
-      <c r="AU65" s="9"/>
-      <c r="AV65" s="9"/>
-      <c r="AW65" s="9"/>
-      <c r="AX65" s="9"/>
-      <c r="AY65" s="9"/>
-      <c r="AZ65" s="9"/>
-      <c r="BA65" s="9"/>
-      <c r="BB65" s="9"/>
-      <c r="BC65" s="9"/>
-      <c r="BD65" s="9"/>
-      <c r="BE65" s="9" t="s">
+      <c r="AK65" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL65" s="13"/>
+      <c r="AM65" s="13"/>
+      <c r="AN65" s="13"/>
+      <c r="AO65" s="13"/>
+      <c r="AP65" s="13"/>
+      <c r="AQ65" s="13"/>
+      <c r="AR65" s="13"/>
+      <c r="AS65" s="13"/>
+      <c r="AT65" s="13"/>
+      <c r="AU65" s="13"/>
+      <c r="AV65" s="13"/>
+      <c r="AW65" s="13"/>
+      <c r="AX65" s="13"/>
+      <c r="AY65" s="13"/>
+      <c r="AZ65" s="13"/>
+      <c r="BA65" s="13"/>
+      <c r="BB65" s="13"/>
+      <c r="BC65" s="13"/>
+      <c r="BD65" s="13"/>
+      <c r="BE65" s="13" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A66" s="11"/>
       <c r="E66" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
@@ -3875,32 +3925,32 @@
       <c r="AL66" s="5"/>
       <c r="AM66" s="5"/>
       <c r="AN66" s="5"/>
-      <c r="AO66" s="5"/>
-      <c r="AP66" s="5"/>
-      <c r="AQ66" s="5"/>
-      <c r="AR66" s="5"/>
-      <c r="AS66" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AT66" s="9"/>
-      <c r="AU66" s="9"/>
-      <c r="AV66" s="9"/>
-      <c r="AW66" s="9"/>
-      <c r="AX66" s="9"/>
-      <c r="AY66" s="9"/>
-      <c r="AZ66" s="9"/>
-      <c r="BA66" s="9"/>
-      <c r="BB66" s="9"/>
-      <c r="BC66" s="9"/>
-      <c r="BD66" s="9"/>
-      <c r="BE66" s="9" t="s">
+      <c r="AO66" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP66" s="13"/>
+      <c r="AQ66" s="13"/>
+      <c r="AR66" s="13"/>
+      <c r="AS66" s="13"/>
+      <c r="AT66" s="13"/>
+      <c r="AU66" s="13"/>
+      <c r="AV66" s="13"/>
+      <c r="AW66" s="13"/>
+      <c r="AX66" s="13"/>
+      <c r="AY66" s="13"/>
+      <c r="AZ66" s="13"/>
+      <c r="BA66" s="13"/>
+      <c r="BB66" s="13"/>
+      <c r="BC66" s="13"/>
+      <c r="BD66" s="13"/>
+      <c r="BE66" s="13" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
       <c r="E67" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
@@ -3941,21 +3991,21 @@
       <c r="AP67" s="5"/>
       <c r="AQ67" s="5"/>
       <c r="AR67" s="5"/>
-      <c r="AS67" s="5"/>
-      <c r="AT67" s="5"/>
-      <c r="AU67" s="5"/>
-      <c r="AV67" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AW67" s="9"/>
-      <c r="AX67" s="9"/>
-      <c r="AY67" s="9"/>
-      <c r="AZ67" s="9"/>
-      <c r="BA67" s="9"/>
-      <c r="BB67" s="9"/>
-      <c r="BC67" s="9"/>
-      <c r="BD67" s="9"/>
-      <c r="BE67" s="9" t="s">
+      <c r="AS67" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="AT67" s="13"/>
+      <c r="AU67" s="13"/>
+      <c r="AV67" s="13"/>
+      <c r="AW67" s="13"/>
+      <c r="AX67" s="13"/>
+      <c r="AY67" s="13"/>
+      <c r="AZ67" s="13"/>
+      <c r="BA67" s="13"/>
+      <c r="BB67" s="13"/>
+      <c r="BC67" s="13"/>
+      <c r="BD67" s="13"/>
+      <c r="BE67" s="13" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4007,29 +4057,86 @@
       <c r="AT68" s="5"/>
       <c r="AU68" s="5"/>
       <c r="AV68" s="5"/>
-      <c r="AW68" s="5"/>
-      <c r="AX68" s="5"/>
-      <c r="AY68" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AZ68" s="9"/>
-      <c r="BA68" s="9"/>
-      <c r="BB68" s="9"/>
-      <c r="BC68" s="9"/>
-      <c r="BD68" s="9"/>
-      <c r="BE68" s="9" t="s">
+      <c r="AW68" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="AX68" s="13"/>
+      <c r="AY68" s="13"/>
+      <c r="AZ68" s="13"/>
+      <c r="BA68" s="13"/>
+      <c r="BB68" s="13"/>
+      <c r="BC68" s="13"/>
+      <c r="BD68" s="13"/>
+      <c r="BE68" s="13" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="69" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="A69" s="11"/>
+      <c r="E69" t="s">
+        <v>83</v>
+      </c>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="5"/>
+      <c r="O69" s="5"/>
+      <c r="P69" s="5"/>
+      <c r="Q69" s="5"/>
+      <c r="R69" s="5"/>
+      <c r="S69" s="5"/>
+      <c r="T69" s="5"/>
+      <c r="U69" s="5"/>
+      <c r="V69" s="5"/>
+      <c r="W69" s="5"/>
+      <c r="X69" s="5"/>
+      <c r="Y69" s="5"/>
+      <c r="Z69" s="5"/>
+      <c r="AA69" s="5"/>
+      <c r="AB69" s="5"/>
+      <c r="AC69" s="5"/>
+      <c r="AD69" s="5"/>
+      <c r="AE69" s="5"/>
+      <c r="AF69" s="5"/>
+      <c r="AG69" s="5"/>
+      <c r="AH69" s="5"/>
+      <c r="AI69" s="5"/>
+      <c r="AJ69" s="5"/>
+      <c r="AK69" s="5"/>
+      <c r="AL69" s="5"/>
+      <c r="AM69" s="5"/>
+      <c r="AN69" s="5"/>
+      <c r="AO69" s="5"/>
+      <c r="AP69" s="5"/>
+      <c r="AQ69" s="5"/>
+      <c r="AR69" s="5"/>
+      <c r="AS69" s="5"/>
+      <c r="AT69" s="5"/>
+      <c r="AU69" s="5"/>
+      <c r="AV69" s="5"/>
+      <c r="AW69" s="5"/>
+      <c r="AX69" s="5"/>
+      <c r="AY69" s="5"/>
+      <c r="AZ69" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="BA69" s="13"/>
+      <c r="BB69" s="13"/>
+      <c r="BC69" s="13"/>
+      <c r="BD69" s="13"/>
+      <c r="BE69" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>5</v>
       </c>
-      <c r="BE69" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="70" spans="1:57" x14ac:dyDescent="0.25">
       <c r="BE70" t="s">
         <v>65</v>
       </c>
@@ -4040,25 +4147,19 @@
       </c>
     </row>
     <row r="72" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="BE72" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="73" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>12</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>1</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E73" t="s">
         <v>13</v>
-      </c>
-      <c r="F72" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE72" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="73" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="E73" t="s">
-        <v>15</v>
       </c>
       <c r="F73" t="s">
         <v>14</v>
@@ -4069,7 +4170,7 @@
     </row>
     <row r="74" spans="1:57" x14ac:dyDescent="0.25">
       <c r="E74" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F74" t="s">
         <v>14</v>
@@ -4080,7 +4181,7 @@
     </row>
     <row r="75" spans="1:57" x14ac:dyDescent="0.25">
       <c r="E75" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F75" t="s">
         <v>14</v>
@@ -4091,7 +4192,7 @@
     </row>
     <row r="76" spans="1:57" x14ac:dyDescent="0.25">
       <c r="E76" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F76" t="s">
         <v>14</v>
@@ -4102,9 +4203,9 @@
     </row>
     <row r="77" spans="1:57" x14ac:dyDescent="0.25">
       <c r="E77" t="s">
-        <v>31</v>
-      </c>
-      <c r="P77" t="s">
+        <v>18</v>
+      </c>
+      <c r="F77" t="s">
         <v>14</v>
       </c>
       <c r="BE77" t="s">
@@ -4113,9 +4214,9 @@
     </row>
     <row r="78" spans="1:57" x14ac:dyDescent="0.25">
       <c r="E78" t="s">
-        <v>32</v>
-      </c>
-      <c r="U78" t="s">
+        <v>31</v>
+      </c>
+      <c r="P78" t="s">
         <v>14</v>
       </c>
       <c r="BE78" t="s">
@@ -4124,7 +4225,7 @@
     </row>
     <row r="79" spans="1:57" x14ac:dyDescent="0.25">
       <c r="E79" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U79" t="s">
         <v>14</v>
@@ -4135,7 +4236,7 @@
     </row>
     <row r="80" spans="1:57" x14ac:dyDescent="0.25">
       <c r="E80" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U80" t="s">
         <v>14</v>
@@ -4146,7 +4247,7 @@
     </row>
     <row r="81" spans="1:57" x14ac:dyDescent="0.25">
       <c r="E81" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U81" t="s">
         <v>14</v>
@@ -4157,9 +4258,9 @@
     </row>
     <row r="82" spans="1:57" x14ac:dyDescent="0.25">
       <c r="E82" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z82" t="s">
+        <v>35</v>
+      </c>
+      <c r="U82" t="s">
         <v>14</v>
       </c>
       <c r="BE82" t="s">
@@ -4168,7 +4269,7 @@
     </row>
     <row r="83" spans="1:57" x14ac:dyDescent="0.25">
       <c r="E83" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Z83" t="s">
         <v>14</v>
@@ -4179,9 +4280,9 @@
     </row>
     <row r="84" spans="1:57" x14ac:dyDescent="0.25">
       <c r="E84" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE84" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z84" t="s">
         <v>14</v>
       </c>
       <c r="BE84" t="s">
@@ -4190,9 +4291,9 @@
     </row>
     <row r="85" spans="1:57" x14ac:dyDescent="0.25">
       <c r="E85" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ85" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE85" t="s">
         <v>14</v>
       </c>
       <c r="BE85" t="s">
@@ -4201,9 +4302,9 @@
     </row>
     <row r="86" spans="1:57" x14ac:dyDescent="0.25">
       <c r="E86" t="s">
-        <v>40</v>
-      </c>
-      <c r="AO86" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ86" t="s">
         <v>14</v>
       </c>
       <c r="BE86" t="s">
@@ -4212,7 +4313,7 @@
     </row>
     <row r="87" spans="1:57" x14ac:dyDescent="0.25">
       <c r="E87" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AO87" t="s">
         <v>14</v>
@@ -4223,9 +4324,9 @@
     </row>
     <row r="88" spans="1:57" x14ac:dyDescent="0.25">
       <c r="E88" t="s">
-        <v>41</v>
-      </c>
-      <c r="AT88" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO88" t="s">
         <v>14</v>
       </c>
       <c r="BE88" t="s">
@@ -4234,7 +4335,7 @@
     </row>
     <row r="89" spans="1:57" x14ac:dyDescent="0.25">
       <c r="E89" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="AT89" t="s">
         <v>14</v>
@@ -4245,34 +4346,45 @@
     </row>
     <row r="90" spans="1:57" x14ac:dyDescent="0.25">
       <c r="E90" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT90" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE90" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="91" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="E91" t="s">
         <v>44</v>
       </c>
-      <c r="BD90" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE90" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="91" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
+      <c r="BD91" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE91" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="92" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
         <v>21</v>
       </c>
-      <c r="L91" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE91" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="92" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="L92" t="s">
+        <v>14</v>
+      </c>
+      <c r="BE92" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="93" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>19</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E93" t="s">
         <v>20</v>
       </c>
-      <c r="F92" t="s">
+      <c r="F93" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>